<commit_message>
Actualizaci[on de datos y de programa 3-dic-22
</commit_message>
<xml_diff>
--- a/Base_Modelo_ARIMAX.xlsx
+++ b/Base_Modelo_ARIMAX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs_Bancolombia\Bancolombia_Argo_2022\Modelos\ARIMAX_Conditional_Forecast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\repos\ARIMAX_Conditional_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC23D1AB-63FC-4316-94FB-71A9065F2B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340BF6A7-3450-482E-BD9B-6585233CF859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11445" yWindow="13380" windowWidth="20730" windowHeight="11160" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +111,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD1D3D4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,12 +153,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,11 +177,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{420B4426-5E36-471D-B25F-3B8E2228384B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,21 +500,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88848EC6-D3A9-432A-B99B-25298BB184AA}">
-  <dimension ref="A1:E271"/>
+  <dimension ref="A1:E290"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B256" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C271" sqref="C271"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -505,7 +531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -522,7 +548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>36526</v>
       </c>
@@ -539,7 +565,7 @@
         <v>168.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>36557</v>
       </c>
@@ -556,7 +582,7 @@
         <v>169.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>36586</v>
       </c>
@@ -573,7 +599,7 @@
         <v>171.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>36617</v>
       </c>
@@ -590,7 +616,7 @@
         <v>171.3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36647</v>
       </c>
@@ -607,7 +633,7 @@
         <v>171.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>36678</v>
       </c>
@@ -624,7 +650,7 @@
         <v>172.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>36708</v>
       </c>
@@ -641,7 +667,7 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>36739</v>
       </c>
@@ -658,7 +684,7 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>36770</v>
       </c>
@@ -675,7 +701,7 @@
         <v>173.7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>36800</v>
       </c>
@@ -692,7 +718,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>36831</v>
       </c>
@@ -709,7 +735,7 @@
         <v>174.1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>36861</v>
       </c>
@@ -726,7 +752,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>36892</v>
       </c>
@@ -743,7 +769,7 @@
         <v>175.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>36923</v>
       </c>
@@ -760,7 +786,7 @@
         <v>175.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>36951</v>
       </c>
@@ -777,7 +803,7 @@
         <v>176.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>36982</v>
       </c>
@@ -794,7 +820,7 @@
         <v>176.9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>37012</v>
       </c>
@@ -811,7 +837,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>37043</v>
       </c>
@@ -828,7 +854,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>37073</v>
       </c>
@@ -845,7 +871,7 @@
         <v>177.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>37104</v>
       </c>
@@ -862,7 +888,7 @@
         <v>177.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>37135</v>
       </c>
@@ -879,7 +905,7 @@
         <v>178.3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>37165</v>
       </c>
@@ -896,7 +922,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>37196</v>
       </c>
@@ -913,7 +939,7 @@
         <v>177.4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>37226</v>
       </c>
@@ -930,7 +956,7 @@
         <v>176.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>37257</v>
       </c>
@@ -947,7 +973,7 @@
         <v>177.1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>37288</v>
       </c>
@@ -964,7 +990,7 @@
         <v>177.8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>37316</v>
       </c>
@@ -981,7 +1007,7 @@
         <v>178.8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>37347</v>
       </c>
@@ -998,7 +1024,7 @@
         <v>179.8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>37377</v>
       </c>
@@ -1015,7 +1041,7 @@
         <v>179.8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>37408</v>
       </c>
@@ -1032,7 +1058,7 @@
         <v>179.9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>37438</v>
       </c>
@@ -1049,7 +1075,7 @@
         <v>180.1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>37469</v>
       </c>
@@ -1066,7 +1092,7 @@
         <v>180.7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>37500</v>
       </c>
@@ -1083,7 +1109,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>37530</v>
       </c>
@@ -1100,7 +1126,7 @@
         <v>181.3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>37561</v>
       </c>
@@ -1117,7 +1143,7 @@
         <v>181.3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37591</v>
       </c>
@@ -1134,7 +1160,7 @@
         <v>180.9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37622</v>
       </c>
@@ -1151,7 +1177,7 @@
         <v>181.7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>37653</v>
       </c>
@@ -1168,7 +1194,7 @@
         <v>183.1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>37681</v>
       </c>
@@ -1185,7 +1211,7 @@
         <v>184.2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>37712</v>
       </c>
@@ -1202,7 +1228,7 @@
         <v>183.8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>37742</v>
       </c>
@@ -1219,7 +1245,7 @@
         <v>183.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>37773</v>
       </c>
@@ -1236,7 +1262,7 @@
         <v>183.7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>37803</v>
       </c>
@@ -1253,7 +1279,7 @@
         <v>183.9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>37834</v>
       </c>
@@ -1270,7 +1296,7 @@
         <v>184.6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>37865</v>
       </c>
@@ -1287,7 +1313,7 @@
         <v>185.2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>37895</v>
       </c>
@@ -1304,7 +1330,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>37926</v>
       </c>
@@ -1321,7 +1347,7 @@
         <v>184.5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>37956</v>
       </c>
@@ -1338,7 +1364,7 @@
         <v>184.3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>37987</v>
       </c>
@@ -1355,7 +1381,7 @@
         <v>185.2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>38018</v>
       </c>
@@ -1372,7 +1398,7 @@
         <v>186.2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>38047</v>
       </c>
@@ -1389,7 +1415,7 @@
         <v>187.4</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>38078</v>
       </c>
@@ -1406,7 +1432,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>38108</v>
       </c>
@@ -1423,7 +1449,7 @@
         <v>189.1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>38139</v>
       </c>
@@ -1440,7 +1466,7 @@
         <v>189.7</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>38169</v>
       </c>
@@ -1457,7 +1483,7 @@
         <v>189.4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>38200</v>
       </c>
@@ -1474,7 +1500,7 @@
         <v>189.5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>38231</v>
       </c>
@@ -1491,7 +1517,7 @@
         <v>189.9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>38261</v>
       </c>
@@ -1508,7 +1534,7 @@
         <v>190.9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>38292</v>
       </c>
@@ -1525,7 +1551,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>38322</v>
       </c>
@@ -1542,7 +1568,7 @@
         <v>190.3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>38353</v>
       </c>
@@ -1559,7 +1585,7 @@
         <v>190.7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>38384</v>
       </c>
@@ -1576,7 +1602,7 @@
         <v>191.8</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>38412</v>
       </c>
@@ -1593,7 +1619,7 @@
         <v>193.3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>38443</v>
       </c>
@@ -1610,7 +1636,7 @@
         <v>194.6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>38473</v>
       </c>
@@ -1627,7 +1653,7 @@
         <v>194.4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>38504</v>
       </c>
@@ -1644,7 +1670,7 @@
         <v>194.5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>38534</v>
       </c>
@@ -1661,7 +1687,7 @@
         <v>195.4</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>38565</v>
       </c>
@@ -1678,7 +1704,7 @@
         <v>196.4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>38596</v>
       </c>
@@ -1695,7 +1721,7 @@
         <v>198.8</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>38626</v>
       </c>
@@ -1712,7 +1738,7 @@
         <v>199.2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>38657</v>
       </c>
@@ -1729,7 +1755,7 @@
         <v>197.6</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>38687</v>
       </c>
@@ -1746,7 +1772,7 @@
         <v>196.8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>38718</v>
       </c>
@@ -1763,7 +1789,7 @@
         <v>198.3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>38749</v>
       </c>
@@ -1780,7 +1806,7 @@
         <v>198.7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>38777</v>
       </c>
@@ -1797,7 +1823,7 @@
         <v>199.8</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>38808</v>
       </c>
@@ -1814,7 +1840,7 @@
         <v>201.5</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>38838</v>
       </c>
@@ -1831,7 +1857,7 @@
         <v>202.5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>38869</v>
       </c>
@@ -1848,7 +1874,7 @@
         <v>202.9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>38899</v>
       </c>
@@ -1865,7 +1891,7 @@
         <v>203.5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>38930</v>
       </c>
@@ -1882,7 +1908,7 @@
         <v>203.9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>38961</v>
       </c>
@@ -1899,7 +1925,7 @@
         <v>202.9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>38991</v>
       </c>
@@ -1916,7 +1942,7 @@
         <v>201.8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>39022</v>
       </c>
@@ -1933,7 +1959,7 @@
         <v>201.5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>39052</v>
       </c>
@@ -1950,7 +1976,7 @@
         <v>201.8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>39083</v>
       </c>
@@ -1967,7 +1993,7 @@
         <v>202.416</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>39114</v>
       </c>
@@ -1984,7 +2010,7 @@
         <v>203.499</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>39142</v>
       </c>
@@ -2001,7 +2027,7 @@
         <v>205.352</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>39173</v>
       </c>
@@ -2018,7 +2044,7 @@
         <v>206.68600000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>39203</v>
       </c>
@@ -2035,7 +2061,7 @@
         <v>207.94900000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>39234</v>
       </c>
@@ -2052,7 +2078,7 @@
         <v>208.352</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>39264</v>
       </c>
@@ -2069,7 +2095,7 @@
         <v>208.29900000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>39295</v>
       </c>
@@ -2086,7 +2112,7 @@
         <v>207.917</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>39326</v>
       </c>
@@ -2103,7 +2129,7 @@
         <v>208.49</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>39356</v>
       </c>
@@ -2120,7 +2146,7 @@
         <v>208.93600000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>39387</v>
       </c>
@@ -2137,7 +2163,7 @@
         <v>210.17699999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>39417</v>
       </c>
@@ -2154,7 +2180,7 @@
         <v>210.036</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>39448</v>
       </c>
@@ -2171,7 +2197,7 @@
         <v>211.08</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>39479</v>
       </c>
@@ -2188,7 +2214,7 @@
         <v>211.69300000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>39508</v>
       </c>
@@ -2205,7 +2231,7 @@
         <v>213.52799999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>39539</v>
       </c>
@@ -2222,7 +2248,7 @@
         <v>214.82300000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>39569</v>
       </c>
@@ -2239,7 +2265,7 @@
         <v>216.63200000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>39600</v>
       </c>
@@ -2256,7 +2282,7 @@
         <v>218.815</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>39630</v>
       </c>
@@ -2273,7 +2299,7 @@
         <v>219.964</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>39661</v>
       </c>
@@ -2290,7 +2316,7 @@
         <v>219.08600000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>39692</v>
       </c>
@@ -2307,7 +2333,7 @@
         <v>218.78299999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>39722</v>
       </c>
@@ -2324,7 +2350,7 @@
         <v>216.57300000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>39753</v>
       </c>
@@ -2341,7 +2367,7 @@
         <v>212.42500000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>39783</v>
       </c>
@@ -2358,7 +2384,7 @@
         <v>210.22800000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>39814</v>
       </c>
@@ -2375,7 +2401,7 @@
         <v>211.143</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>39845</v>
       </c>
@@ -2392,7 +2418,7 @@
         <v>212.19300000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>39873</v>
       </c>
@@ -2409,7 +2435,7 @@
         <v>212.709</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>39904</v>
       </c>
@@ -2426,7 +2452,7 @@
         <v>213.24</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>39934</v>
       </c>
@@ -2443,7 +2469,7 @@
         <v>213.85599999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>39965</v>
       </c>
@@ -2460,7 +2486,7 @@
         <v>215.69300000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>39995</v>
       </c>
@@ -2477,7 +2503,7 @@
         <v>215.351</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>40026</v>
       </c>
@@ -2494,7 +2520,7 @@
         <v>215.834</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>40057</v>
       </c>
@@ -2511,7 +2537,7 @@
         <v>215.96899999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>40087</v>
       </c>
@@ -2528,7 +2554,7 @@
         <v>216.17699999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>40118</v>
       </c>
@@ -2545,7 +2571,7 @@
         <v>216.33</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>40148</v>
       </c>
@@ -2562,7 +2588,7 @@
         <v>215.94900000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>40179</v>
       </c>
@@ -2579,7 +2605,7 @@
         <v>216.68700000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>40210</v>
       </c>
@@ -2596,7 +2622,7 @@
         <v>216.74100000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>40238</v>
       </c>
@@ -2613,7 +2639,7 @@
         <v>217.631</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>40269</v>
       </c>
@@ -2630,7 +2656,7 @@
         <v>218.00899999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>40299</v>
       </c>
@@ -2647,7 +2673,7 @@
         <v>218.178</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>40330</v>
       </c>
@@ -2664,7 +2690,7 @@
         <v>217.965</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>40360</v>
       </c>
@@ -2681,7 +2707,7 @@
         <v>218.011</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>40391</v>
       </c>
@@ -2698,7 +2724,7 @@
         <v>218.31200000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>40422</v>
       </c>
@@ -2715,7 +2741,7 @@
         <v>218.43899999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>40452</v>
       </c>
@@ -2732,7 +2758,7 @@
         <v>218.71100000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>40483</v>
       </c>
@@ -2749,7 +2775,7 @@
         <v>218.803</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>40513</v>
       </c>
@@ -2766,7 +2792,7 @@
         <v>219.179</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>40544</v>
       </c>
@@ -2783,7 +2809,7 @@
         <v>220.22300000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>40575</v>
       </c>
@@ -2800,7 +2826,7 @@
         <v>221.309</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>40603</v>
       </c>
@@ -2817,7 +2843,7 @@
         <v>223.46700000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>40634</v>
       </c>
@@ -2834,7 +2860,7 @@
         <v>224.90600000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>40664</v>
       </c>
@@ -2851,7 +2877,7 @@
         <v>225.964</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>40695</v>
       </c>
@@ -2868,7 +2894,7 @@
         <v>225.72200000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>40725</v>
       </c>
@@ -2885,7 +2911,7 @@
         <v>225.922</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>40756</v>
       </c>
@@ -2902,7 +2928,7 @@
         <v>226.54499999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>40787</v>
       </c>
@@ -2919,7 +2945,7 @@
         <v>226.88900000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>40817</v>
       </c>
@@ -2936,7 +2962,7 @@
         <v>226.42099999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>40848</v>
       </c>
@@ -2953,7 +2979,7 @@
         <v>226.23</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>40878</v>
       </c>
@@ -2970,7 +2996,7 @@
         <v>225.672</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>40909</v>
       </c>
@@ -2987,7 +3013,7 @@
         <v>226.66499999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>40940</v>
       </c>
@@ -3004,7 +3030,7 @@
         <v>227.66300000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>40969</v>
       </c>
@@ -3021,7 +3047,7 @@
         <v>229.392</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>41000</v>
       </c>
@@ -3038,7 +3064,7 @@
         <v>230.08500000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>41030</v>
       </c>
@@ -3055,7 +3081,7 @@
         <v>229.815</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>41061</v>
       </c>
@@ -3072,7 +3098,7 @@
         <v>229.47800000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>41091</v>
       </c>
@@ -3089,7 +3115,7 @@
         <v>229.10400000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>41122</v>
       </c>
@@ -3106,7 +3132,7 @@
         <v>230.37899999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>41153</v>
       </c>
@@ -3123,7 +3149,7 @@
         <v>231.40700000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>41183</v>
       </c>
@@ -3140,7 +3166,7 @@
         <v>231.31700000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>41214</v>
       </c>
@@ -3157,7 +3183,7 @@
         <v>230.221</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>41244</v>
       </c>
@@ -3174,7 +3200,7 @@
         <v>229.601</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>41275</v>
       </c>
@@ -3191,7 +3217,7 @@
         <v>230.28</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>41306</v>
       </c>
@@ -3208,7 +3234,7 @@
         <v>232.166</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>41334</v>
       </c>
@@ -3225,7 +3251,7 @@
         <v>232.773</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>41365</v>
       </c>
@@ -3242,7 +3268,7 @@
         <v>232.53100000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>41395</v>
       </c>
@@ -3259,7 +3285,7 @@
         <v>232.94499999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>41426</v>
       </c>
@@ -3276,7 +3302,7 @@
         <v>233.50399999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>41456</v>
       </c>
@@ -3293,7 +3319,7 @@
         <v>233.596</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>41487</v>
       </c>
@@ -3310,7 +3336,7 @@
         <v>233.87700000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>41518</v>
       </c>
@@ -3327,7 +3353,7 @@
         <v>234.149</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>41548</v>
       </c>
@@ -3344,7 +3370,7 @@
         <v>233.54599999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>41579</v>
       </c>
@@ -3361,7 +3387,7 @@
         <v>233.06899999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>41609</v>
       </c>
@@ -3378,7 +3404,7 @@
         <v>233.04900000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>41640</v>
       </c>
@@ -3395,7 +3421,7 @@
         <v>233.916</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>41671</v>
       </c>
@@ -3412,7 +3438,7 @@
         <v>234.78100000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>41699</v>
       </c>
@@ -3429,7 +3455,7 @@
         <v>236.29300000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>41730</v>
       </c>
@@ -3446,7 +3472,7 @@
         <v>237.072</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>41760</v>
       </c>
@@ -3463,7 +3489,7 @@
         <v>237.9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>41791</v>
       </c>
@@ -3480,7 +3506,7 @@
         <v>238.34299999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>41821</v>
       </c>
@@ -3497,7 +3523,7 @@
         <v>238.25</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>41852</v>
       </c>
@@ -3514,7 +3540,7 @@
         <v>237.852</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>41883</v>
       </c>
@@ -3531,7 +3557,7 @@
         <v>238.03100000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>41913</v>
       </c>
@@ -3548,7 +3574,7 @@
         <v>237.43299999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>41944</v>
       </c>
@@ -3565,7 +3591,7 @@
         <v>236.15100000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>41974</v>
       </c>
@@ -3582,7 +3608,7 @@
         <v>234.81200000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>42005</v>
       </c>
@@ -3599,7 +3625,7 @@
         <v>233.70699999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>42036</v>
       </c>
@@ -3616,7 +3642,7 @@
         <v>234.72200000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>42064</v>
       </c>
@@ -3633,7 +3659,7 @@
         <v>236.119</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>42095</v>
       </c>
@@ -3650,7 +3676,7 @@
         <v>236.59899999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>42125</v>
       </c>
@@ -3667,7 +3693,7 @@
         <v>237.80500000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>42156</v>
       </c>
@@ -3684,7 +3710,7 @@
         <v>238.63800000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>42186</v>
       </c>
@@ -3701,7 +3727,7 @@
         <v>238.654</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>42217</v>
       </c>
@@ -3718,7 +3744,7 @@
         <v>238.316</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>42248</v>
       </c>
@@ -3735,7 +3761,7 @@
         <v>237.94499999999999</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>42278</v>
       </c>
@@ -3752,7 +3778,7 @@
         <v>237.83799999999999</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>42309</v>
       </c>
@@ -3769,7 +3795,7 @@
         <v>237.33600000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>42339</v>
       </c>
@@ -3786,7 +3812,7 @@
         <v>236.52500000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>42370</v>
       </c>
@@ -3803,7 +3829,7 @@
         <v>236.916</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>42401</v>
       </c>
@@ -3820,7 +3846,7 @@
         <v>237.11099999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>42430</v>
       </c>
@@ -3837,7 +3863,7 @@
         <v>238.13200000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>42461</v>
       </c>
@@ -3854,7 +3880,7 @@
         <v>239.261</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>42491</v>
       </c>
@@ -3871,7 +3897,7 @@
         <v>240.22900000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>42522</v>
       </c>
@@ -3888,7 +3914,7 @@
         <v>241.018</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>42552</v>
       </c>
@@ -3905,7 +3931,7 @@
         <v>240.62799999999999</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>42583</v>
       </c>
@@ -3922,7 +3948,7 @@
         <v>240.84899999999999</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>42614</v>
       </c>
@@ -3939,7 +3965,7 @@
         <v>241.428</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>42644</v>
       </c>
@@ -3956,7 +3982,7 @@
         <v>241.72900000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>42675</v>
       </c>
@@ -3973,7 +3999,7 @@
         <v>241.35300000000001</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>42705</v>
       </c>
@@ -3990,7 +4016,7 @@
         <v>241.43199999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>42736</v>
       </c>
@@ -4007,7 +4033,7 @@
         <v>242.839</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>42767</v>
       </c>
@@ -4024,7 +4050,7 @@
         <v>243.60300000000001</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>42795</v>
       </c>
@@ -4041,7 +4067,7 @@
         <v>243.80099999999999</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>42826</v>
       </c>
@@ -4058,7 +4084,7 @@
         <v>244.524</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>42856</v>
       </c>
@@ -4075,7 +4101,7 @@
         <v>244.733</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>42887</v>
       </c>
@@ -4092,7 +4118,7 @@
         <v>244.95500000000001</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>42917</v>
       </c>
@@ -4109,7 +4135,7 @@
         <v>244.786</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>42948</v>
       </c>
@@ -4126,7 +4152,7 @@
         <v>245.51900000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>42979</v>
       </c>
@@ -4143,7 +4169,7 @@
         <v>246.81899999999999</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>43009</v>
       </c>
@@ -4160,7 +4186,7 @@
         <v>246.66300000000001</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>43040</v>
       </c>
@@ -4177,7 +4203,7 @@
         <v>246.66900000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>43070</v>
       </c>
@@ -4194,7 +4220,7 @@
         <v>246.524</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>43101</v>
       </c>
@@ -4211,7 +4237,7 @@
         <v>247.86699999999999</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>43132</v>
       </c>
@@ -4228,7 +4254,7 @@
         <v>248.99100000000001</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>43160</v>
       </c>
@@ -4245,7 +4271,7 @@
         <v>249.554</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>43191</v>
       </c>
@@ -4262,7 +4288,7 @@
         <v>250.54599999999999</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>43221</v>
       </c>
@@ -4279,7 +4305,7 @@
         <v>251.58799999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>43252</v>
       </c>
@@ -4296,7 +4322,7 @@
         <v>251.989</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>43282</v>
       </c>
@@ -4313,7 +4339,7 @@
         <v>252.006</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>43313</v>
       </c>
@@ -4330,7 +4356,7 @@
         <v>252.14599999999999</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>43344</v>
       </c>
@@ -4347,7 +4373,7 @@
         <v>252.43899999999999</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>43374</v>
       </c>
@@ -4364,7 +4390,7 @@
         <v>252.88499999999999</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>43405</v>
       </c>
@@ -4381,7 +4407,7 @@
         <v>252.03800000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>43435</v>
       </c>
@@ -4398,7 +4424,7 @@
         <v>251.233</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>43466</v>
       </c>
@@ -4415,7 +4441,7 @@
         <v>251.71199999999999</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>43497</v>
       </c>
@@ -4432,7 +4458,7 @@
         <v>252.77600000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>43525</v>
       </c>
@@ -4449,7 +4475,7 @@
         <v>254.202</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>43556</v>
       </c>
@@ -4466,7 +4492,7 @@
         <v>255.548</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>43586</v>
       </c>
@@ -4483,7 +4509,7 @@
         <v>256.09199999999998</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>43617</v>
       </c>
@@ -4500,7 +4526,7 @@
         <v>256.14299999999997</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>43647</v>
       </c>
@@ -4517,7 +4543,7 @@
         <v>256.57100000000003</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>43678</v>
       </c>
@@ -4534,7 +4560,7 @@
         <v>256.55799999999999</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>43709</v>
       </c>
@@ -4551,7 +4577,7 @@
         <v>256.75900000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>43739</v>
       </c>
@@ -4568,7 +4594,7 @@
         <v>257.346</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>43770</v>
       </c>
@@ -4585,7 +4611,7 @@
         <v>257.20800000000003</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>43800</v>
       </c>
@@ -4602,7 +4628,7 @@
         <v>256.97399999999999</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>43831</v>
       </c>
@@ -4619,7 +4645,7 @@
         <v>257.971</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>43862</v>
       </c>
@@ -4636,7 +4662,7 @@
         <v>258.678</v>
       </c>
     </row>
-    <row r="245" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>43891</v>
       </c>
@@ -4653,7 +4679,7 @@
         <v>258.11500000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>43922</v>
       </c>
@@ -4670,7 +4696,7 @@
         <v>256.38900000000001</v>
       </c>
     </row>
-    <row r="247" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>43952</v>
       </c>
@@ -4687,7 +4713,7 @@
         <v>256.39400000000001</v>
       </c>
     </row>
-    <row r="248" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>43983</v>
       </c>
@@ -4704,7 +4730,7 @@
         <v>257.79700000000003</v>
       </c>
     </row>
-    <row r="249" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>44013</v>
       </c>
@@ -4721,7 +4747,7 @@
         <v>259.101</v>
       </c>
     </row>
-    <row r="250" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>44044</v>
       </c>
@@ -4738,7 +4764,7 @@
         <v>259.91800000000001</v>
       </c>
     </row>
-    <row r="251" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>44075</v>
       </c>
@@ -4755,7 +4781,7 @@
         <v>260.27999999999997</v>
       </c>
     </row>
-    <row r="252" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>44105</v>
       </c>
@@ -4772,7 +4798,7 @@
         <v>260.38799999999998</v>
       </c>
     </row>
-    <row r="253" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>44136</v>
       </c>
@@ -4789,7 +4815,7 @@
         <v>260.22899999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>44166</v>
       </c>
@@ -4806,7 +4832,7 @@
         <v>260.47399999999999</v>
       </c>
     </row>
-    <row r="255" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>44197</v>
       </c>
@@ -4823,7 +4849,7 @@
         <v>261.58199999999999</v>
       </c>
     </row>
-    <row r="256" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>44228</v>
       </c>
@@ -4840,7 +4866,7 @@
         <v>263.01400000000001</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>44256</v>
       </c>
@@ -4857,7 +4883,7 @@
         <v>264.87700000000001</v>
       </c>
     </row>
-    <row r="258" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>44287</v>
       </c>
@@ -4874,7 +4900,7 @@
         <v>267.05399999999997</v>
       </c>
     </row>
-    <row r="259" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>44317</v>
       </c>
@@ -4891,7 +4917,7 @@
         <v>269.19499999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>44348</v>
       </c>
@@ -4908,7 +4934,7 @@
         <v>271.69600000000003</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>44378</v>
       </c>
@@ -4925,7 +4951,7 @@
         <v>273.00299999999999</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>44409</v>
       </c>
@@ -4942,7 +4968,7 @@
         <v>273.56700000000001</v>
       </c>
     </row>
-    <row r="263" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>44440</v>
       </c>
@@ -4959,7 +4985,7 @@
         <v>274.31</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>44470</v>
       </c>
@@ -4976,7 +5002,7 @@
         <v>276.589</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>44501</v>
       </c>
@@ -4993,7 +5019,7 @@
         <v>277.94799999999998</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>44531</v>
       </c>
@@ -5010,7 +5036,7 @@
         <v>278.80200000000002</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>44562</v>
       </c>
@@ -5027,7 +5053,7 @@
         <v>281.14800000000002</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>44593</v>
       </c>
@@ -5044,7 +5070,7 @@
         <v>283.71600000000001</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>44621</v>
       </c>
@@ -5061,7 +5087,7 @@
         <v>287.50400000000002</v>
       </c>
     </row>
-    <row r="270" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>44652</v>
       </c>
@@ -5078,7 +5104,7 @@
         <v>289.10899999999998</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>44682</v>
       </c>
@@ -5094,6 +5120,146 @@
       <c r="E271" s="5">
         <v>292.29599999999999</v>
       </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A272" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B272" s="5">
+        <v>119.31</v>
+      </c>
+      <c r="C272" s="5">
+        <v>122.7</v>
+      </c>
+      <c r="D272" s="5">
+        <v>104.1</v>
+      </c>
+      <c r="E272" s="5">
+        <v>296.3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A273" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B273" s="5">
+        <v>120.27</v>
+      </c>
+      <c r="C273" s="5">
+        <v>111.9</v>
+      </c>
+      <c r="D273" s="5">
+        <v>104.8</v>
+      </c>
+      <c r="E273" s="5">
+        <v>296.3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A274" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B274" s="5">
+        <v>121.5</v>
+      </c>
+      <c r="C274" s="5">
+        <v>100.5</v>
+      </c>
+      <c r="D274" s="5">
+        <v>104.7</v>
+      </c>
+      <c r="E274" s="5">
+        <v>296.2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A275" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B275" s="5">
+        <v>122.63</v>
+      </c>
+      <c r="C275" s="5">
+        <v>89.8</v>
+      </c>
+      <c r="D275" s="5">
+        <v>104.8</v>
+      </c>
+      <c r="E275" s="5">
+        <v>296.8</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A276" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B276" s="5">
+        <v>123.51</v>
+      </c>
+      <c r="C276" s="5">
+        <v>93.3</v>
+      </c>
+      <c r="D276" s="5">
+        <v>104.7</v>
+      </c>
+      <c r="E276" s="5">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C277" s="5"/>
+      <c r="D277" s="5"/>
+      <c r="E277" s="5"/>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C281" s="5"/>
+      <c r="D281" s="5"/>
+      <c r="E281" s="5"/>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C282" s="5"/>
+      <c r="D282" s="5"/>
+      <c r="E282" s="5"/>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C283" s="5"/>
+      <c r="D283" s="5"/>
+      <c r="E283" s="5"/>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C284" s="5"/>
+      <c r="D284" s="5"/>
+      <c r="E284" s="5"/>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C285" s="5"/>
+      <c r="D285" s="5"/>
+      <c r="E285" s="5"/>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C286" s="5"/>
+      <c r="D286" s="5"/>
+      <c r="E286" s="5"/>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C287" s="5"/>
+      <c r="D287" s="5"/>
+      <c r="E287" s="5"/>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C288" s="5"/>
+      <c r="D288" s="5"/>
+      <c r="E288" s="5"/>
+    </row>
+    <row r="289" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C289" s="5"/>
+      <c r="D289" s="5"/>
+      <c r="E289" s="5"/>
+    </row>
+    <row r="290" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C290" s="5"/>
+      <c r="D290" s="5"/>
+      <c r="E290" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5112,18 +5278,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C921DE1D-2686-44DF-B218-59946BA2C5A6}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
@@ -5134,7 +5300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -5148,270 +5314,200 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44713</v>
-      </c>
-      <c r="B4" s="2">
-        <v>107</v>
-      </c>
-      <c r="C4" s="2">
-        <v>106.64749999999998</v>
-      </c>
-      <c r="D4" s="2">
-        <v>290.06128788618037</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>44866</v>
+      </c>
+      <c r="B4" s="7">
+        <v>93</v>
+      </c>
+      <c r="C4" s="8">
+        <v>105.28570000000001</v>
+      </c>
+      <c r="D4" s="8">
+        <v>299.55200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44743</v>
-      </c>
-      <c r="B5" s="2">
-        <v>105</v>
-      </c>
-      <c r="C5" s="2">
-        <v>106.82039999999999</v>
-      </c>
-      <c r="D5" s="2">
-        <v>290.58705157503749</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>44896</v>
+      </c>
+      <c r="B5" s="7">
+        <v>93</v>
+      </c>
+      <c r="C5" s="8">
+        <v>105.12909999999999</v>
+      </c>
+      <c r="D5" s="8">
+        <v>300.49369999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44774</v>
-      </c>
-      <c r="B6" s="2">
-        <v>104</v>
-      </c>
-      <c r="C6" s="2">
-        <v>107.18909999999998</v>
-      </c>
-      <c r="D6" s="2">
-        <v>291.00978626799764</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>44927</v>
+      </c>
+      <c r="B6" s="7">
+        <v>93</v>
+      </c>
+      <c r="C6" s="8">
+        <v>104.63590000000001</v>
+      </c>
+      <c r="D6" s="8">
+        <v>301.19729999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44805</v>
-      </c>
-      <c r="B7" s="2">
-        <v>103</v>
-      </c>
-      <c r="C7" s="2">
-        <v>107.55699999999997</v>
-      </c>
-      <c r="D7" s="2">
-        <v>291.44829787319395</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>44958</v>
+      </c>
+      <c r="B7" s="7">
+        <v>94</v>
+      </c>
+      <c r="C7" s="8">
+        <v>104.3762</v>
+      </c>
+      <c r="D7" s="8">
+        <v>301.95159999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44835</v>
-      </c>
-      <c r="B8" s="2">
-        <v>102</v>
-      </c>
-      <c r="C8" s="2">
-        <v>107.93029999999999</v>
-      </c>
-      <c r="D8" s="2">
-        <v>292.46274260891573</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>44986</v>
+      </c>
+      <c r="B8" s="7">
+        <v>94</v>
+      </c>
+      <c r="C8" s="8">
+        <v>104.14279999999999</v>
+      </c>
+      <c r="D8" s="8">
+        <v>302.65159999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44866</v>
-      </c>
-      <c r="B9" s="2">
-        <v>102</v>
-      </c>
-      <c r="C9" s="2">
-        <v>108.2915</v>
-      </c>
-      <c r="D9" s="2">
-        <v>292.63705942037308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>45017</v>
+      </c>
+      <c r="B9" s="7">
+        <v>94</v>
+      </c>
+      <c r="C9" s="8">
+        <v>103.82980000000001</v>
+      </c>
+      <c r="D9" s="8">
+        <v>303.20440000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44896</v>
-      </c>
-      <c r="B10" s="2">
-        <v>101</v>
-      </c>
-      <c r="C10" s="2">
-        <v>108.64710000000001</v>
-      </c>
-      <c r="D10" s="2">
-        <v>292.51925825092991</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>45047</v>
+      </c>
+      <c r="B10" s="7">
+        <v>94</v>
+      </c>
+      <c r="C10" s="8">
+        <v>103.7283</v>
+      </c>
+      <c r="D10" s="8">
+        <v>303.8655</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>44927</v>
-      </c>
-      <c r="B11" s="2">
-        <v>101</v>
-      </c>
-      <c r="C11" s="2">
-        <v>108.98250000000002</v>
-      </c>
-      <c r="D11" s="2">
-        <v>293.51187852149275</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>45078</v>
+      </c>
+      <c r="B11" s="7">
+        <v>94</v>
+      </c>
+      <c r="C11" s="8">
+        <v>103.7323</v>
+      </c>
+      <c r="D11" s="8">
+        <v>304.54219999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>44958</v>
-      </c>
-      <c r="B12" s="2">
-        <v>99</v>
-      </c>
-      <c r="C12" s="2">
-        <v>109.33760000000001</v>
-      </c>
-      <c r="D12" s="2">
-        <v>294.37878650583082</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+        <v>45108</v>
+      </c>
+      <c r="B12" s="7">
+        <v>95</v>
+      </c>
+      <c r="C12" s="8">
+        <v>103.9573</v>
+      </c>
+      <c r="D12" s="8">
+        <v>305.19690000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44986</v>
-      </c>
-      <c r="B13" s="2">
+        <v>45139</v>
+      </c>
+      <c r="B13" s="7">
+        <v>96</v>
+      </c>
+      <c r="C13" s="8">
+        <v>104.08620000000001</v>
+      </c>
+      <c r="D13" s="8">
+        <v>305.9325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B14" s="7">
+        <v>97</v>
+      </c>
+      <c r="C14" s="8">
+        <v>104.2342</v>
+      </c>
+      <c r="D14" s="8">
+        <v>306.71159999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B15" s="7">
+        <v>97</v>
+      </c>
+      <c r="C15" s="8">
+        <v>104.4456</v>
+      </c>
+      <c r="D15" s="8">
+        <v>307.6277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B16" s="7">
         <v>98</v>
       </c>
-      <c r="C13" s="2">
-        <v>109.69790000000003</v>
-      </c>
-      <c r="D13" s="2">
-        <v>295.16446447648315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>45017</v>
-      </c>
-      <c r="B14" s="2">
-        <v>97</v>
-      </c>
-      <c r="C14" s="2">
-        <v>110.06850000000003</v>
-      </c>
-      <c r="D14" s="2">
-        <v>297.64167142081999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>45047</v>
-      </c>
-      <c r="B15" s="2">
-        <v>97</v>
-      </c>
-      <c r="C15" s="2">
-        <v>110.43530000000003</v>
-      </c>
-      <c r="D15" s="2">
-        <v>300.35400068038177</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>45078</v>
-      </c>
-      <c r="B16" s="2">
-        <v>96</v>
-      </c>
-      <c r="C16" s="2">
-        <v>110.80330000000002</v>
-      </c>
-      <c r="D16" s="2">
-        <v>297.71536294366229</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C16" s="8">
+        <v>104.59869999999999</v>
+      </c>
+      <c r="D16" s="8">
+        <v>308.42380000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45108</v>
-      </c>
-      <c r="B17" s="2">
-        <v>96</v>
-      </c>
-      <c r="C17" s="2">
-        <v>111.23530000000002</v>
-      </c>
-      <c r="D17" s="2">
-        <v>298.55355081011373</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>45139</v>
-      </c>
-      <c r="B18" s="2">
-        <v>96</v>
-      </c>
-      <c r="C18" s="2">
-        <v>111.55900000000003</v>
-      </c>
-      <c r="D18" s="2">
-        <v>298.76575311250423</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>45170</v>
-      </c>
-      <c r="B19" s="2">
-        <v>96</v>
-      </c>
-      <c r="C19" s="2">
-        <v>111.83690000000003</v>
-      </c>
-      <c r="D19" s="2">
-        <v>298.89660454973125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>45200</v>
-      </c>
-      <c r="B20" s="2">
-        <v>97</v>
-      </c>
-      <c r="C20" s="2">
-        <v>111.97970000000001</v>
-      </c>
-      <c r="D20" s="2">
-        <v>299.28931792761847</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B21" s="2">
-        <v>97</v>
-      </c>
-      <c r="C21" s="2">
-        <v>112.23320000000001</v>
-      </c>
-      <c r="D21" s="2">
-        <v>299.1292055506886</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
         <v>45261</v>
       </c>
-      <c r="B22" s="2">
-        <v>97</v>
-      </c>
-      <c r="C22" s="2">
-        <v>112.5081</v>
-      </c>
-      <c r="D22" s="2">
-        <v>298.74698346958155</v>
+      <c r="B17" s="7">
+        <v>98</v>
+      </c>
+      <c r="C17" s="8">
+        <v>104.73779999999999</v>
+      </c>
+      <c r="D17" s="8">
+        <v>309.19330000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización base de datos
</commit_message>
<xml_diff>
--- a/Base_Modelo_ARIMAX.xlsx
+++ b/Base_Modelo_ARIMAX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\repos\ARIMAX_Conditional_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340BF6A7-3450-482E-BD9B-6585233CF859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B91C9-5327-4560-B881-A88A644F9995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
   </bookViews>
@@ -503,10 +503,10 @@
   <dimension ref="A1:E290"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B261" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B283" sqref="B283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +559,7 @@
         <v>25.51</v>
       </c>
       <c r="D3" s="4">
-        <v>91.794200000000004</v>
+        <v>91.4251</v>
       </c>
       <c r="E3" s="4">
         <v>168.8</v>
@@ -576,7 +576,7 @@
         <v>27.78</v>
       </c>
       <c r="D4" s="4">
-        <v>92.127200000000002</v>
+        <v>91.735699999999994</v>
       </c>
       <c r="E4" s="4">
         <v>169.8</v>
@@ -593,7 +593,7 @@
         <v>27.49</v>
       </c>
       <c r="D5" s="4">
-        <v>92.473299999999995</v>
+        <v>92.093299999999999</v>
       </c>
       <c r="E5" s="4">
         <v>171.2</v>
@@ -610,7 +610,7 @@
         <v>22.76</v>
       </c>
       <c r="D6" s="4">
-        <v>93.061899999999994</v>
+        <v>92.683800000000005</v>
       </c>
       <c r="E6" s="4">
         <v>171.3</v>
@@ -627,7 +627,7 @@
         <v>27.74</v>
       </c>
       <c r="D7" s="4">
-        <v>93.342699999999994</v>
+        <v>92.937600000000003</v>
       </c>
       <c r="E7" s="4">
         <v>171.5</v>
@@ -644,7 +644,7 @@
         <v>29.8</v>
       </c>
       <c r="D8" s="4">
-        <v>93.390799999999999</v>
+        <v>93.007599999999996</v>
       </c>
       <c r="E8" s="4">
         <v>172.4</v>
@@ -661,7 +661,7 @@
         <v>28.68</v>
       </c>
       <c r="D9" s="4">
-        <v>93.203999999999994</v>
+        <v>92.845799999999997</v>
       </c>
       <c r="E9" s="4">
         <v>172.8</v>
@@ -678,7 +678,7 @@
         <v>30.2</v>
       </c>
       <c r="D10" s="4">
-        <v>92.963700000000003</v>
+        <v>92.597200000000001</v>
       </c>
       <c r="E10" s="4">
         <v>172.8</v>
@@ -695,7 +695,7 @@
         <v>33.14</v>
       </c>
       <c r="D11" s="4">
-        <v>93.353300000000004</v>
+        <v>92.965299999999999</v>
       </c>
       <c r="E11" s="4">
         <v>173.7</v>
@@ -712,7 +712,7 @@
         <v>30.96</v>
       </c>
       <c r="D12" s="4">
-        <v>93.001900000000006</v>
+        <v>92.641800000000003</v>
       </c>
       <c r="E12" s="4">
         <v>174</v>
@@ -729,7 +729,7 @@
         <v>32.549999999999997</v>
       </c>
       <c r="D13" s="4">
-        <v>93.0137</v>
+        <v>92.661799999999999</v>
       </c>
       <c r="E13" s="4">
         <v>174.1</v>
@@ -746,7 +746,7 @@
         <v>25.66</v>
       </c>
       <c r="D14" s="4">
-        <v>92.738799999999998</v>
+        <v>92.3459</v>
       </c>
       <c r="E14" s="4">
         <v>174</v>
@@ -763,7 +763,7 @@
         <v>25.62</v>
       </c>
       <c r="D15" s="4">
-        <v>92.205399999999997</v>
+        <v>91.890299999999996</v>
       </c>
       <c r="E15" s="4">
         <v>175.1</v>
@@ -780,7 +780,7 @@
         <v>27.5</v>
       </c>
       <c r="D16" s="4">
-        <v>91.581299999999999</v>
+        <v>91.291499999999999</v>
       </c>
       <c r="E16" s="4">
         <v>175.8</v>
@@ -797,7 +797,7 @@
         <v>24.5</v>
       </c>
       <c r="D17" s="4">
-        <v>91.356700000000004</v>
+        <v>91.052599999999998</v>
       </c>
       <c r="E17" s="4">
         <v>176.2</v>
@@ -814,7 +814,7 @@
         <v>25.66</v>
       </c>
       <c r="D18" s="4">
-        <v>91.072000000000003</v>
+        <v>90.729299999999995</v>
       </c>
       <c r="E18" s="4">
         <v>176.9</v>
@@ -831,7 +831,7 @@
         <v>28.31</v>
       </c>
       <c r="D19" s="4">
-        <v>90.533500000000004</v>
+        <v>90.2577</v>
       </c>
       <c r="E19" s="4">
         <v>177.7</v>
@@ -848,7 +848,7 @@
         <v>27.85</v>
       </c>
       <c r="D20" s="4">
-        <v>90.032200000000003</v>
+        <v>89.767700000000005</v>
       </c>
       <c r="E20" s="4">
         <v>178</v>
@@ -865,7 +865,7 @@
         <v>24.61</v>
       </c>
       <c r="D21" s="4">
-        <v>89.477800000000002</v>
+        <v>89.225999999999999</v>
       </c>
       <c r="E21" s="4">
         <v>177.5</v>
@@ -882,7 +882,7 @@
         <v>25.68</v>
       </c>
       <c r="D22" s="4">
-        <v>89.383799999999994</v>
+        <v>89.132599999999996</v>
       </c>
       <c r="E22" s="4">
         <v>177.5</v>
@@ -899,7 +899,7 @@
         <v>25.62</v>
       </c>
       <c r="D23" s="4">
-        <v>88.926199999999994</v>
+        <v>88.667900000000003</v>
       </c>
       <c r="E23" s="4">
         <v>178.3</v>
@@ -916,7 +916,7 @@
         <v>20.54</v>
       </c>
       <c r="D24" s="4">
-        <v>88.636499999999998</v>
+        <v>88.392600000000002</v>
       </c>
       <c r="E24" s="4">
         <v>177.7</v>
@@ -933,7 +933,7 @@
         <v>18.8</v>
       </c>
       <c r="D25" s="4">
-        <v>88.105800000000002</v>
+        <v>87.877399999999994</v>
       </c>
       <c r="E25" s="4">
         <v>177.4</v>
@@ -950,7 +950,7 @@
         <v>18.71</v>
       </c>
       <c r="D26" s="4">
-        <v>88.089699999999993</v>
+        <v>87.834400000000002</v>
       </c>
       <c r="E26" s="4">
         <v>176.7</v>
@@ -967,7 +967,7 @@
         <v>19.420000000000002</v>
       </c>
       <c r="D27" s="4">
-        <v>88.670599999999993</v>
+        <v>88.466499999999996</v>
       </c>
       <c r="E27" s="4">
         <v>177.1</v>
@@ -984,7 +984,7 @@
         <v>20.28</v>
       </c>
       <c r="D28" s="4">
-        <v>88.672300000000007</v>
+        <v>88.466099999999997</v>
       </c>
       <c r="E28" s="4">
         <v>177.8</v>
@@ -1001,7 +1001,7 @@
         <v>23.7</v>
       </c>
       <c r="D29" s="4">
-        <v>89.362399999999994</v>
+        <v>89.122799999999998</v>
       </c>
       <c r="E29" s="4">
         <v>178.8</v>
@@ -1018,7 +1018,7 @@
         <v>25.73</v>
       </c>
       <c r="D30" s="4">
-        <v>89.793300000000002</v>
+        <v>89.553200000000004</v>
       </c>
       <c r="E30" s="4">
         <v>179.8</v>
@@ -1035,7 +1035,7 @@
         <v>25.35</v>
       </c>
       <c r="D31" s="4">
-        <v>90.162899999999993</v>
+        <v>89.933999999999997</v>
       </c>
       <c r="E31" s="4">
         <v>179.8</v>
@@ -1052,7 +1052,7 @@
         <v>24.08</v>
       </c>
       <c r="D32" s="4">
-        <v>90.907799999999995</v>
+        <v>90.676900000000003</v>
       </c>
       <c r="E32" s="4">
         <v>179.9</v>
@@ -1069,7 +1069,7 @@
         <v>25.74</v>
       </c>
       <c r="D33" s="4">
-        <v>90.876099999999994</v>
+        <v>90.645499999999998</v>
       </c>
       <c r="E33" s="4">
         <v>180.1</v>
@@ -1086,7 +1086,7 @@
         <v>26.65</v>
       </c>
       <c r="D34" s="4">
-        <v>90.784999999999997</v>
+        <v>90.547499999999999</v>
       </c>
       <c r="E34" s="4">
         <v>180.7</v>
@@ -1103,7 +1103,7 @@
         <v>28.4</v>
       </c>
       <c r="D35" s="4">
-        <v>90.893100000000004</v>
+        <v>90.638099999999994</v>
       </c>
       <c r="E35" s="4">
         <v>181</v>
@@ -1120,7 +1120,7 @@
         <v>27.54</v>
       </c>
       <c r="D36" s="4">
-        <v>90.628900000000002</v>
+        <v>90.4041</v>
       </c>
       <c r="E36" s="4">
         <v>181.3</v>
@@ -1137,7 +1137,7 @@
         <v>24.34</v>
       </c>
       <c r="D37" s="4">
-        <v>91.136600000000001</v>
+        <v>90.898499999999999</v>
       </c>
       <c r="E37" s="4">
         <v>181.3</v>
@@ -1154,7 +1154,7 @@
         <v>28.33</v>
       </c>
       <c r="D38" s="4">
-        <v>90.6374</v>
+        <v>90.388999999999996</v>
       </c>
       <c r="E38" s="4">
         <v>180.9</v>
@@ -1171,7 +1171,7 @@
         <v>31.18</v>
       </c>
       <c r="D39" s="4">
-        <v>91.385199999999998</v>
+        <v>91.135499999999993</v>
       </c>
       <c r="E39" s="4">
         <v>181.7</v>
@@ -1188,7 +1188,7 @@
         <v>32.770000000000003</v>
       </c>
       <c r="D40" s="4">
-        <v>91.494</v>
+        <v>91.250200000000007</v>
       </c>
       <c r="E40" s="4">
         <v>183.1</v>
@@ -1205,7 +1205,7 @@
         <v>30.61</v>
       </c>
       <c r="D41" s="4">
-        <v>91.221000000000004</v>
+        <v>91.005899999999997</v>
       </c>
       <c r="E41" s="4">
         <v>184.2</v>
@@ -1222,7 +1222,7 @@
         <v>25</v>
       </c>
       <c r="D42" s="4">
-        <v>90.644800000000004</v>
+        <v>90.428100000000001</v>
       </c>
       <c r="E42" s="4">
         <v>183.8</v>
@@ -1239,7 +1239,7 @@
         <v>25.86</v>
       </c>
       <c r="D43" s="4">
-        <v>90.616299999999995</v>
+        <v>90.407300000000006</v>
       </c>
       <c r="E43" s="4">
         <v>183.5</v>
@@ -1256,7 +1256,7 @@
         <v>27.65</v>
       </c>
       <c r="D44" s="4">
-        <v>90.737200000000001</v>
+        <v>90.521799999999999</v>
       </c>
       <c r="E44" s="4">
         <v>183.7</v>
@@ -1273,7 +1273,7 @@
         <v>28.35</v>
       </c>
       <c r="D45" s="4">
-        <v>91.202799999999996</v>
+        <v>90.989599999999996</v>
       </c>
       <c r="E45" s="4">
         <v>183.9</v>
@@ -1290,7 +1290,7 @@
         <v>29.89</v>
       </c>
       <c r="D46" s="4">
-        <v>91.011899999999997</v>
+        <v>90.785799999999995</v>
       </c>
       <c r="E46" s="4">
         <v>184.6</v>
@@ -1307,7 +1307,7 @@
         <v>27.11</v>
       </c>
       <c r="D47" s="4">
-        <v>91.635499999999993</v>
+        <v>91.382900000000006</v>
       </c>
       <c r="E47" s="4">
         <v>185.2</v>
@@ -1324,7 +1324,7 @@
         <v>29.61</v>
       </c>
       <c r="D48" s="4">
-        <v>91.737200000000001</v>
+        <v>91.500500000000002</v>
       </c>
       <c r="E48" s="4">
         <v>185</v>
@@ -1341,7 +1341,7 @@
         <v>28.75</v>
       </c>
       <c r="D49" s="4">
-        <v>92.350499999999997</v>
+        <v>92.126499999999993</v>
       </c>
       <c r="E49" s="4">
         <v>184.5</v>
@@ -1358,7 +1358,7 @@
         <v>29.81</v>
       </c>
       <c r="D50" s="4">
-        <v>92.401899999999998</v>
+        <v>92.172200000000004</v>
       </c>
       <c r="E50" s="4">
         <v>184.3</v>
@@ -1375,7 +1375,7 @@
         <v>31.28</v>
       </c>
       <c r="D51" s="4">
-        <v>92.564300000000003</v>
+        <v>92.326999999999998</v>
       </c>
       <c r="E51" s="4">
         <v>185.2</v>
@@ -1392,7 +1392,7 @@
         <v>30.86</v>
       </c>
       <c r="D52" s="4">
-        <v>93.109200000000001</v>
+        <v>92.887299999999996</v>
       </c>
       <c r="E52" s="4">
         <v>186.2</v>
@@ -1409,7 +1409,7 @@
         <v>33.630000000000003</v>
       </c>
       <c r="D53" s="4">
-        <v>92.740300000000005</v>
+        <v>92.532499999999999</v>
       </c>
       <c r="E53" s="4">
         <v>187.4</v>
@@ -1426,7 +1426,7 @@
         <v>33.590000000000003</v>
       </c>
       <c r="D54" s="4">
-        <v>93.125500000000002</v>
+        <v>92.909599999999998</v>
       </c>
       <c r="E54" s="4">
         <v>188</v>
@@ -1443,7 +1443,7 @@
         <v>37.57</v>
       </c>
       <c r="D55" s="4">
-        <v>93.796999999999997</v>
+        <v>93.583799999999997</v>
       </c>
       <c r="E55" s="4">
         <v>189.1</v>
@@ -1460,7 +1460,7 @@
         <v>35.18</v>
       </c>
       <c r="D56" s="4">
-        <v>93.067700000000002</v>
+        <v>92.862099999999998</v>
       </c>
       <c r="E56" s="4">
         <v>189.7</v>
@@ -1477,7 +1477,7 @@
         <v>38.22</v>
       </c>
       <c r="D57" s="4">
-        <v>93.764600000000002</v>
+        <v>93.551100000000005</v>
       </c>
       <c r="E57" s="4">
         <v>189.4</v>
@@ -1494,7 +1494,7 @@
         <v>42.74</v>
       </c>
       <c r="D58" s="4">
-        <v>93.851600000000005</v>
+        <v>93.632800000000003</v>
       </c>
       <c r="E58" s="4">
         <v>189.5</v>
@@ -1511,7 +1511,7 @@
         <v>43.2</v>
       </c>
       <c r="D59" s="4">
-        <v>93.939300000000003</v>
+        <v>93.741799999999998</v>
       </c>
       <c r="E59" s="4">
         <v>189.9</v>
@@ -1528,7 +1528,7 @@
         <v>49.78</v>
       </c>
       <c r="D60" s="4">
-        <v>94.801199999999994</v>
+        <v>94.567099999999996</v>
       </c>
       <c r="E60" s="4">
         <v>190.9</v>
@@ -1545,7 +1545,7 @@
         <v>43.11</v>
       </c>
       <c r="D61" s="4">
-        <v>95.037899999999993</v>
+        <v>94.8</v>
       </c>
       <c r="E61" s="4">
         <v>191</v>
@@ -1562,7 +1562,7 @@
         <v>39.6</v>
       </c>
       <c r="D62" s="4">
-        <v>95.743300000000005</v>
+        <v>95.542599999999993</v>
       </c>
       <c r="E62" s="4">
         <v>190.3</v>
@@ -1579,7 +1579,7 @@
         <v>44.51</v>
       </c>
       <c r="D63" s="4">
-        <v>96.116399999999999</v>
+        <v>95.883099999999999</v>
       </c>
       <c r="E63" s="4">
         <v>190.7</v>
@@ -1596,7 +1596,7 @@
         <v>45.48</v>
       </c>
       <c r="D64" s="4">
-        <v>96.82</v>
+        <v>96.561599999999999</v>
       </c>
       <c r="E64" s="4">
         <v>191.8</v>
@@ -1613,7 +1613,7 @@
         <v>53.1</v>
       </c>
       <c r="D65" s="4">
-        <v>96.672499999999999</v>
+        <v>96.437100000000001</v>
       </c>
       <c r="E65" s="4">
         <v>193.3</v>
@@ -1630,7 +1630,7 @@
         <v>51.88</v>
       </c>
       <c r="D66" s="4">
-        <v>96.863799999999998</v>
+        <v>96.628</v>
       </c>
       <c r="E66" s="4">
         <v>194.6</v>
@@ -1647,7 +1647,7 @@
         <v>48.65</v>
       </c>
       <c r="D67" s="4">
-        <v>96.962199999999996</v>
+        <v>96.730599999999995</v>
       </c>
       <c r="E67" s="4">
         <v>194.4</v>
@@ -1664,7 +1664,7 @@
         <v>54.35</v>
       </c>
       <c r="D68" s="4">
-        <v>97.352999999999994</v>
+        <v>97.148799999999994</v>
       </c>
       <c r="E68" s="4">
         <v>194.5</v>
@@ -1681,7 +1681,7 @@
         <v>57.52</v>
       </c>
       <c r="D69" s="4">
-        <v>97.042500000000004</v>
+        <v>96.838300000000004</v>
       </c>
       <c r="E69" s="4">
         <v>195.4</v>
@@ -1698,7 +1698,7 @@
         <v>63.98</v>
       </c>
       <c r="D70" s="4">
-        <v>97.385599999999997</v>
+        <v>97.160300000000007</v>
       </c>
       <c r="E70" s="4">
         <v>196.4</v>
@@ -1715,7 +1715,7 @@
         <v>62.91</v>
       </c>
       <c r="D71" s="4">
-        <v>95.509</v>
+        <v>95.272900000000007</v>
       </c>
       <c r="E71" s="4">
         <v>198.8</v>
@@ -1732,7 +1732,7 @@
         <v>58.54</v>
       </c>
       <c r="D72" s="4">
-        <v>96.644499999999994</v>
+        <v>96.438299999999998</v>
       </c>
       <c r="E72" s="4">
         <v>199.2</v>
@@ -1749,7 +1749,7 @@
         <v>55.24</v>
       </c>
       <c r="D73" s="4">
-        <v>97.673599999999993</v>
+        <v>97.495099999999994</v>
       </c>
       <c r="E73" s="4">
         <v>197.6</v>
@@ -1766,7 +1766,7 @@
         <v>56.86</v>
       </c>
       <c r="D74" s="4">
-        <v>98.210800000000006</v>
+        <v>97.978800000000007</v>
       </c>
       <c r="E74" s="4">
         <v>196.8</v>
@@ -1783,7 +1783,7 @@
         <v>62.99</v>
       </c>
       <c r="D75" s="4">
-        <v>98.335300000000004</v>
+        <v>98.130499999999998</v>
       </c>
       <c r="E75" s="4">
         <v>198.3</v>
@@ -1800,7 +1800,7 @@
         <v>60.21</v>
       </c>
       <c r="D76" s="4">
-        <v>98.341200000000001</v>
+        <v>98.177899999999994</v>
       </c>
       <c r="E76" s="4">
         <v>198.7</v>
@@ -1817,7 +1817,7 @@
         <v>62.06</v>
       </c>
       <c r="D77" s="4">
-        <v>98.591499999999996</v>
+        <v>98.389799999999994</v>
       </c>
       <c r="E77" s="4">
         <v>199.8</v>
@@ -1834,7 +1834,7 @@
         <v>70.260000000000005</v>
       </c>
       <c r="D78" s="4">
-        <v>98.904200000000003</v>
+        <v>98.676900000000003</v>
       </c>
       <c r="E78" s="4">
         <v>201.5</v>
@@ -1851,7 +1851,7 @@
         <v>69.78</v>
       </c>
       <c r="D79" s="4">
-        <v>98.899900000000002</v>
+        <v>98.705200000000005</v>
       </c>
       <c r="E79" s="4">
         <v>202.5</v>
@@ -1868,7 +1868,7 @@
         <v>68.56</v>
       </c>
       <c r="D80" s="4">
-        <v>99.209000000000003</v>
+        <v>99.042699999999996</v>
       </c>
       <c r="E80" s="4">
         <v>202.9</v>
@@ -1885,7 +1885,7 @@
         <v>73.67</v>
       </c>
       <c r="D81" s="4">
-        <v>99.147300000000001</v>
+        <v>98.980400000000003</v>
       </c>
       <c r="E81" s="4">
         <v>203.5</v>
@@ -1902,7 +1902,7 @@
         <v>73.23</v>
       </c>
       <c r="D82" s="4">
-        <v>99.581500000000005</v>
+        <v>99.410600000000002</v>
       </c>
       <c r="E82" s="4">
         <v>203.9</v>
@@ -1919,7 +1919,7 @@
         <v>61.96</v>
       </c>
       <c r="D83" s="4">
-        <v>99.413300000000007</v>
+        <v>99.220699999999994</v>
       </c>
       <c r="E83" s="4">
         <v>202.9</v>
@@ -1936,7 +1936,7 @@
         <v>57.81</v>
       </c>
       <c r="D84" s="4">
-        <v>99.293099999999995</v>
+        <v>99.125299999999996</v>
       </c>
       <c r="E84" s="4">
         <v>201.8</v>
@@ -1953,7 +1953,7 @@
         <v>58.76</v>
       </c>
       <c r="D85" s="4">
-        <v>99.2376</v>
+        <v>99.096900000000005</v>
       </c>
       <c r="E85" s="4">
         <v>201.5</v>
@@ -1970,7 +1970,7 @@
         <v>62.47</v>
       </c>
       <c r="D86" s="4">
-        <v>100.2526</v>
+        <v>100.1122</v>
       </c>
       <c r="E86" s="4">
         <v>201.8</v>
@@ -1987,7 +1987,7 @@
         <v>53.68</v>
       </c>
       <c r="D87" s="4">
-        <v>99.86</v>
+        <v>99.757099999999994</v>
       </c>
       <c r="E87" s="4">
         <v>202.416</v>
@@ -2004,7 +2004,7 @@
         <v>57.56</v>
       </c>
       <c r="D88" s="4">
-        <v>100.8096</v>
+        <v>100.72750000000001</v>
       </c>
       <c r="E88" s="4">
         <v>203.499</v>
@@ -2021,7 +2021,7 @@
         <v>62.05</v>
       </c>
       <c r="D89" s="4">
-        <v>101.0257</v>
+        <v>100.9023</v>
       </c>
       <c r="E89" s="4">
         <v>205.352</v>
@@ -2038,7 +2038,7 @@
         <v>67.489999999999995</v>
       </c>
       <c r="D90" s="4">
-        <v>101.7497</v>
+        <v>101.5874</v>
       </c>
       <c r="E90" s="4">
         <v>206.68600000000001</v>
@@ -2055,7 +2055,7 @@
         <v>67.209999999999994</v>
       </c>
       <c r="D91" s="4">
-        <v>101.81480000000001</v>
+        <v>101.62990000000001</v>
       </c>
       <c r="E91" s="4">
         <v>207.94900000000001</v>
@@ -2072,7 +2072,7 @@
         <v>71.05</v>
       </c>
       <c r="D92" s="4">
-        <v>101.8424</v>
+        <v>101.6482</v>
       </c>
       <c r="E92" s="4">
         <v>208.352</v>
@@ -2089,7 +2089,7 @@
         <v>76.930000000000007</v>
       </c>
       <c r="D93" s="4">
-        <v>101.7209</v>
+        <v>101.49250000000001</v>
       </c>
       <c r="E93" s="4">
         <v>208.29900000000001</v>
@@ -2106,7 +2106,7 @@
         <v>70.760000000000005</v>
       </c>
       <c r="D94" s="4">
-        <v>101.9639</v>
+        <v>101.6874</v>
       </c>
       <c r="E94" s="4">
         <v>207.917</v>
@@ -2123,7 +2123,7 @@
         <v>77.17</v>
       </c>
       <c r="D95" s="4">
-        <v>102.20229999999999</v>
+        <v>101.93980000000001</v>
       </c>
       <c r="E95" s="4">
         <v>208.49</v>
@@ -2140,7 +2140,7 @@
         <v>82.34</v>
       </c>
       <c r="D96" s="4">
-        <v>101.8873</v>
+        <v>101.6345</v>
       </c>
       <c r="E96" s="4">
         <v>208.93600000000001</v>
@@ -2157,7 +2157,7 @@
         <v>92.41</v>
       </c>
       <c r="D97" s="4">
-        <v>102.4717</v>
+        <v>102.2068</v>
       </c>
       <c r="E97" s="4">
         <v>210.17699999999999</v>
@@ -2174,7 +2174,7 @@
         <v>90.93</v>
       </c>
       <c r="D98" s="4">
-        <v>102.46210000000001</v>
+        <v>102.2604</v>
       </c>
       <c r="E98" s="4">
         <v>210.036</v>
@@ -2191,7 +2191,7 @@
         <v>92.18</v>
       </c>
       <c r="D99" s="4">
-        <v>102.31480000000001</v>
+        <v>102.14</v>
       </c>
       <c r="E99" s="4">
         <v>211.08</v>
@@ -2208,7 +2208,7 @@
         <v>94.99</v>
       </c>
       <c r="D100" s="4">
-        <v>101.9384</v>
+        <v>101.7671</v>
       </c>
       <c r="E100" s="4">
         <v>211.69300000000001</v>
@@ -2225,7 +2225,7 @@
         <v>103.64</v>
       </c>
       <c r="D101" s="4">
-        <v>101.5904</v>
+        <v>101.4355</v>
       </c>
       <c r="E101" s="4">
         <v>213.52799999999999</v>
@@ -2242,7 +2242,7 @@
         <v>109.07</v>
       </c>
       <c r="D102" s="4">
-        <v>100.9098</v>
+        <v>100.7424</v>
       </c>
       <c r="E102" s="4">
         <v>214.82300000000001</v>
@@ -2259,7 +2259,7 @@
         <v>122.8</v>
       </c>
       <c r="D103" s="4">
-        <v>100.3073</v>
+        <v>100.13200000000001</v>
       </c>
       <c r="E103" s="4">
         <v>216.63200000000001</v>
@@ -2276,7 +2276,7 @@
         <v>132.32</v>
       </c>
       <c r="D104" s="4">
-        <v>100.0853</v>
+        <v>99.865099999999998</v>
       </c>
       <c r="E104" s="4">
         <v>218.815</v>
@@ -2293,7 +2293,7 @@
         <v>132.72</v>
       </c>
       <c r="D105" s="4">
-        <v>99.612399999999994</v>
+        <v>99.421400000000006</v>
       </c>
       <c r="E105" s="4">
         <v>219.964</v>
@@ -2310,7 +2310,7 @@
         <v>113.24</v>
       </c>
       <c r="D106" s="4">
-        <v>98.060100000000006</v>
+        <v>97.844800000000006</v>
       </c>
       <c r="E106" s="4">
         <v>219.08600000000001</v>
@@ -2327,7 +2327,7 @@
         <v>97.23</v>
       </c>
       <c r="D107" s="4">
-        <v>93.845100000000002</v>
+        <v>93.558999999999997</v>
       </c>
       <c r="E107" s="4">
         <v>218.78299999999999</v>
@@ -2344,7 +2344,7 @@
         <v>71.58</v>
       </c>
       <c r="D108" s="4">
-        <v>94.703599999999994</v>
+        <v>94.495599999999996</v>
       </c>
       <c r="E108" s="4">
         <v>216.57300000000001</v>
@@ -2361,7 +2361,7 @@
         <v>52.45</v>
       </c>
       <c r="D109" s="4">
-        <v>93.473699999999994</v>
+        <v>93.268900000000002</v>
       </c>
       <c r="E109" s="4">
         <v>212.42500000000001</v>
@@ -2378,7 +2378,7 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D110" s="4">
-        <v>90.825000000000003</v>
+        <v>90.628</v>
       </c>
       <c r="E110" s="4">
         <v>210.22800000000001</v>
@@ -2395,7 +2395,7 @@
         <v>43.44</v>
       </c>
       <c r="D111" s="4">
-        <v>88.582999999999998</v>
+        <v>88.381100000000004</v>
       </c>
       <c r="E111" s="4">
         <v>211.143</v>
@@ -2412,7 +2412,7 @@
         <v>43.32</v>
       </c>
       <c r="D112" s="4">
-        <v>88.006900000000002</v>
+        <v>87.841200000000001</v>
       </c>
       <c r="E112" s="4">
         <v>212.19300000000001</v>
@@ -2429,7 +2429,7 @@
         <v>46.54</v>
       </c>
       <c r="D113" s="4">
-        <v>86.604500000000002</v>
+        <v>86.479399999999998</v>
       </c>
       <c r="E113" s="4">
         <v>212.709</v>
@@ -2446,7 +2446,7 @@
         <v>50.18</v>
       </c>
       <c r="D114" s="4">
-        <v>85.940600000000003</v>
+        <v>85.788300000000007</v>
       </c>
       <c r="E114" s="4">
         <v>213.24</v>
@@ -2463,7 +2463,7 @@
         <v>57.3</v>
       </c>
       <c r="D115" s="4">
-        <v>85.063500000000005</v>
+        <v>84.951599999999999</v>
       </c>
       <c r="E115" s="4">
         <v>213.85599999999999</v>
@@ -2480,7 +2480,7 @@
         <v>68.61</v>
       </c>
       <c r="D116" s="4">
-        <v>84.784099999999995</v>
+        <v>84.692800000000005</v>
       </c>
       <c r="E116" s="4">
         <v>215.69300000000001</v>
@@ -2497,7 +2497,7 @@
         <v>64.44</v>
       </c>
       <c r="D117" s="4">
-        <v>85.747100000000003</v>
+        <v>85.704400000000007</v>
       </c>
       <c r="E117" s="4">
         <v>215.351</v>
@@ -2514,7 +2514,7 @@
         <v>72.510000000000005</v>
       </c>
       <c r="D118" s="4">
-        <v>86.709400000000002</v>
+        <v>86.661699999999996</v>
       </c>
       <c r="E118" s="4">
         <v>215.834</v>
@@ -2531,7 +2531,7 @@
         <v>67.650000000000006</v>
       </c>
       <c r="D119" s="4">
-        <v>87.407200000000003</v>
+        <v>87.403300000000002</v>
       </c>
       <c r="E119" s="4">
         <v>215.96899999999999</v>
@@ -2548,7 +2548,7 @@
         <v>72.77</v>
       </c>
       <c r="D120" s="4">
-        <v>87.659499999999994</v>
+        <v>87.603499999999997</v>
       </c>
       <c r="E120" s="4">
         <v>216.17699999999999</v>
@@ -2565,7 +2565,7 @@
         <v>76.66</v>
       </c>
       <c r="D121" s="4">
-        <v>88.006100000000004</v>
+        <v>87.9559</v>
       </c>
       <c r="E121" s="4">
         <v>216.33</v>
@@ -2582,7 +2582,7 @@
         <v>74.459999999999994</v>
       </c>
       <c r="D122" s="4">
-        <v>88.281899999999993</v>
+        <v>88.246799999999993</v>
       </c>
       <c r="E122" s="4">
         <v>215.94900000000001</v>
@@ -2599,7 +2599,7 @@
         <v>76.17</v>
       </c>
       <c r="D123" s="4">
-        <v>89.2744</v>
+        <v>89.191100000000006</v>
       </c>
       <c r="E123" s="4">
         <v>216.68700000000001</v>
@@ -2616,7 +2616,7 @@
         <v>73.75</v>
       </c>
       <c r="D124" s="4">
-        <v>89.564800000000005</v>
+        <v>89.497200000000007</v>
       </c>
       <c r="E124" s="4">
         <v>216.74100000000001</v>
@@ -2633,7 +2633,7 @@
         <v>78.83</v>
       </c>
       <c r="D125" s="4">
-        <v>90.229600000000005</v>
+        <v>90.141900000000007</v>
       </c>
       <c r="E125" s="4">
         <v>217.631</v>
@@ -2650,7 +2650,7 @@
         <v>84.82</v>
       </c>
       <c r="D126" s="4">
-        <v>90.568899999999999</v>
+        <v>90.459100000000007</v>
       </c>
       <c r="E126" s="4">
         <v>218.00899999999999</v>
@@ -2667,7 +2667,7 @@
         <v>75.95</v>
       </c>
       <c r="D127" s="4">
-        <v>91.824700000000007</v>
+        <v>91.701999999999998</v>
       </c>
       <c r="E127" s="4">
         <v>218.178</v>
@@ -2684,7 +2684,7 @@
         <v>74.760000000000005</v>
       </c>
       <c r="D128" s="4">
-        <v>92.007000000000005</v>
+        <v>91.899699999999996</v>
       </c>
       <c r="E128" s="4">
         <v>217.965</v>
@@ -2701,7 +2701,7 @@
         <v>75.58</v>
       </c>
       <c r="D129" s="4">
-        <v>92.396699999999996</v>
+        <v>92.252200000000002</v>
       </c>
       <c r="E129" s="4">
         <v>218.011</v>
@@ -2718,7 +2718,7 @@
         <v>77.040000000000006</v>
       </c>
       <c r="D130" s="4">
-        <v>92.711799999999997</v>
+        <v>92.5899</v>
       </c>
       <c r="E130" s="4">
         <v>218.31200000000001</v>
@@ -2735,7 +2735,7 @@
         <v>77.84</v>
       </c>
       <c r="D131" s="4">
-        <v>92.925200000000004</v>
+        <v>92.856399999999994</v>
       </c>
       <c r="E131" s="4">
         <v>218.43899999999999</v>
@@ -2752,7 +2752,7 @@
         <v>82.67</v>
       </c>
       <c r="D132" s="4">
-        <v>92.711500000000001</v>
+        <v>92.603700000000003</v>
       </c>
       <c r="E132" s="4">
         <v>218.71100000000001</v>
@@ -2769,7 +2769,7 @@
         <v>85.28</v>
       </c>
       <c r="D133" s="4">
-        <v>92.753500000000003</v>
+        <v>92.677300000000002</v>
       </c>
       <c r="E133" s="4">
         <v>218.803</v>
@@ -2786,7 +2786,7 @@
         <v>91.45</v>
       </c>
       <c r="D134" s="4">
-        <v>93.649199999999993</v>
+        <v>93.585099999999997</v>
       </c>
       <c r="E134" s="4">
         <v>219.179</v>
@@ -2803,7 +2803,7 @@
         <v>96.52</v>
       </c>
       <c r="D135" s="4">
-        <v>93.476799999999997</v>
+        <v>93.394400000000005</v>
       </c>
       <c r="E135" s="4">
         <v>220.22300000000001</v>
@@ -2820,7 +2820,7 @@
         <v>103.72</v>
       </c>
       <c r="D136" s="4">
-        <v>93.061700000000002</v>
+        <v>92.992999999999995</v>
       </c>
       <c r="E136" s="4">
         <v>221.309</v>
@@ -2837,7 +2837,7 @@
         <v>114.64</v>
       </c>
       <c r="D137" s="4">
-        <v>94.0244</v>
+        <v>93.981999999999999</v>
       </c>
       <c r="E137" s="4">
         <v>223.46700000000001</v>
@@ -2854,7 +2854,7 @@
         <v>123.26</v>
       </c>
       <c r="D138" s="4">
-        <v>93.701099999999997</v>
+        <v>93.652500000000003</v>
       </c>
       <c r="E138" s="4">
         <v>224.90600000000001</v>
@@ -2871,7 +2871,7 @@
         <v>114.99</v>
       </c>
       <c r="D139" s="4">
-        <v>93.849000000000004</v>
+        <v>93.777500000000003</v>
       </c>
       <c r="E139" s="4">
         <v>225.964</v>
@@ -2888,7 +2888,7 @@
         <v>113.83</v>
       </c>
       <c r="D140" s="4">
-        <v>94.084400000000002</v>
+        <v>94.046700000000001</v>
       </c>
       <c r="E140" s="4">
         <v>225.72200000000001</v>
@@ -2905,7 +2905,7 @@
         <v>116.97</v>
       </c>
       <c r="D141" s="4">
-        <v>94.588099999999997</v>
+        <v>94.493099999999998</v>
       </c>
       <c r="E141" s="4">
         <v>225.922</v>
@@ -2922,7 +2922,7 @@
         <v>110.22</v>
       </c>
       <c r="D142" s="4">
-        <v>95.160499999999999</v>
+        <v>95.096900000000005</v>
       </c>
       <c r="E142" s="4">
         <v>226.54499999999999</v>
@@ -2939,7 +2939,7 @@
         <v>112.83</v>
       </c>
       <c r="D143" s="4">
-        <v>95.085499999999996</v>
+        <v>95.028099999999995</v>
       </c>
       <c r="E143" s="4">
         <v>226.88900000000001</v>
@@ -2956,7 +2956,7 @@
         <v>109.55</v>
       </c>
       <c r="D144" s="4">
-        <v>95.690200000000004</v>
+        <v>95.692400000000006</v>
       </c>
       <c r="E144" s="4">
         <v>226.42099999999999</v>
@@ -2973,7 +2973,7 @@
         <v>110.77</v>
       </c>
       <c r="D145" s="4">
-        <v>95.730699999999999</v>
+        <v>95.691299999999998</v>
       </c>
       <c r="E145" s="4">
         <v>226.23</v>
@@ -2990,7 +2990,7 @@
         <v>107.87</v>
       </c>
       <c r="D146" s="4">
-        <v>96.204700000000003</v>
+        <v>96.193799999999996</v>
       </c>
       <c r="E146" s="4">
         <v>225.672</v>
@@ -3007,7 +3007,7 @@
         <v>110.69</v>
       </c>
       <c r="D147" s="4">
-        <v>96.777199999999993</v>
+        <v>96.778999999999996</v>
       </c>
       <c r="E147" s="4">
         <v>226.66499999999999</v>
@@ -3024,7 +3024,7 @@
         <v>119.33</v>
       </c>
       <c r="D148" s="4">
-        <v>97.051000000000002</v>
+        <v>97.0959</v>
       </c>
       <c r="E148" s="4">
         <v>227.66300000000001</v>
@@ -3041,7 +3041,7 @@
         <v>125.45</v>
       </c>
       <c r="D149" s="4">
-        <v>96.571399999999997</v>
+        <v>96.591899999999995</v>
       </c>
       <c r="E149" s="4">
         <v>229.392</v>
@@ -3058,7 +3058,7 @@
         <v>119.75</v>
       </c>
       <c r="D150" s="4">
-        <v>97.313900000000004</v>
+        <v>97.294200000000004</v>
       </c>
       <c r="E150" s="4">
         <v>230.08500000000001</v>
@@ -3075,7 +3075,7 @@
         <v>110.34</v>
       </c>
       <c r="D151" s="4">
-        <v>97.466899999999995</v>
+        <v>97.485299999999995</v>
       </c>
       <c r="E151" s="4">
         <v>229.815</v>
@@ -3092,7 +3092,7 @@
         <v>95.16</v>
       </c>
       <c r="D152" s="4">
-        <v>97.457700000000003</v>
+        <v>97.495900000000006</v>
       </c>
       <c r="E152" s="4">
         <v>229.47800000000001</v>
@@ -3109,7 +3109,7 @@
         <v>102.62</v>
       </c>
       <c r="D153" s="4">
-        <v>97.678600000000003</v>
+        <v>97.6922</v>
       </c>
       <c r="E153" s="4">
         <v>229.10400000000001</v>
@@ -3126,7 +3126,7 @@
         <v>113.36</v>
       </c>
       <c r="D154" s="4">
-        <v>97.284199999999998</v>
+        <v>97.306100000000001</v>
       </c>
       <c r="E154" s="4">
         <v>230.37899999999999</v>
@@ -3143,7 +3143,7 @@
         <v>112.86</v>
       </c>
       <c r="D155" s="4">
-        <v>97.229500000000002</v>
+        <v>97.238299999999995</v>
       </c>
       <c r="E155" s="4">
         <v>231.40700000000001</v>
@@ -3160,7 +3160,7 @@
         <v>111.71</v>
       </c>
       <c r="D156" s="4">
-        <v>97.534400000000005</v>
+        <v>97.542500000000004</v>
       </c>
       <c r="E156" s="4">
         <v>231.31700000000001</v>
@@ -3177,7 +3177,7 @@
         <v>109.06</v>
       </c>
       <c r="D157" s="4">
-        <v>97.983699999999999</v>
+        <v>97.933999999999997</v>
       </c>
       <c r="E157" s="4">
         <v>230.221</v>
@@ -3194,7 +3194,7 @@
         <v>109.49</v>
       </c>
       <c r="D158" s="4">
-        <v>98.212199999999996</v>
+        <v>98.198400000000007</v>
       </c>
       <c r="E158" s="4">
         <v>229.601</v>
@@ -3211,7 +3211,7 @@
         <v>112.96</v>
       </c>
       <c r="D159" s="4">
-        <v>98.166399999999996</v>
+        <v>98.2029</v>
       </c>
       <c r="E159" s="4">
         <v>230.28</v>
@@ -3228,7 +3228,7 @@
         <v>116.05</v>
       </c>
       <c r="D160" s="4">
-        <v>98.645799999999994</v>
+        <v>98.673299999999998</v>
       </c>
       <c r="E160" s="4">
         <v>232.166</v>
@@ -3245,7 +3245,7 @@
         <v>108.47</v>
       </c>
       <c r="D161" s="4">
-        <v>99.059700000000007</v>
+        <v>99.078800000000001</v>
       </c>
       <c r="E161" s="4">
         <v>232.773</v>
@@ -3262,7 +3262,7 @@
         <v>102.25</v>
       </c>
       <c r="D162" s="4">
-        <v>98.992699999999999</v>
+        <v>98.965800000000002</v>
       </c>
       <c r="E162" s="4">
         <v>232.53100000000001</v>
@@ -3279,7 +3279,7 @@
         <v>102.56</v>
       </c>
       <c r="D163" s="4">
-        <v>99.072599999999994</v>
+        <v>99.056700000000006</v>
       </c>
       <c r="E163" s="4">
         <v>232.94499999999999</v>
@@ -3296,7 +3296,7 @@
         <v>102.92</v>
       </c>
       <c r="D164" s="4">
-        <v>99.206500000000005</v>
+        <v>99.242400000000004</v>
       </c>
       <c r="E164" s="4">
         <v>233.50399999999999</v>
@@ -3313,7 +3313,7 @@
         <v>107.93</v>
       </c>
       <c r="D165" s="4">
-        <v>98.920400000000001</v>
+        <v>98.925799999999995</v>
       </c>
       <c r="E165" s="4">
         <v>233.596</v>
@@ -3330,7 +3330,7 @@
         <v>111.28</v>
       </c>
       <c r="D166" s="4">
-        <v>99.499600000000001</v>
+        <v>99.505899999999997</v>
       </c>
       <c r="E166" s="4">
         <v>233.87700000000001</v>
@@ -3347,7 +3347,7 @@
         <v>111.6</v>
       </c>
       <c r="D167" s="4">
-        <v>100.0568</v>
+        <v>100.0391</v>
       </c>
       <c r="E167" s="4">
         <v>234.149</v>
@@ -3364,7 +3364,7 @@
         <v>109.08</v>
       </c>
       <c r="D168" s="4">
-        <v>99.916799999999995</v>
+        <v>99.920299999999997</v>
       </c>
       <c r="E168" s="4">
         <v>233.54599999999999</v>
@@ -3381,7 +3381,7 @@
         <v>107.79</v>
       </c>
       <c r="D169" s="4">
-        <v>100.17619999999999</v>
+        <v>100.1661</v>
       </c>
       <c r="E169" s="4">
         <v>233.06899999999999</v>
@@ -3398,7 +3398,7 @@
         <v>110.76</v>
       </c>
       <c r="D170" s="4">
-        <v>100.36579999999999</v>
+        <v>100.3777</v>
       </c>
       <c r="E170" s="4">
         <v>233.04900000000001</v>
@@ -3415,7 +3415,7 @@
         <v>108.12</v>
       </c>
       <c r="D171" s="4">
-        <v>100.038</v>
+        <v>99.998999999999995</v>
       </c>
       <c r="E171" s="4">
         <v>233.916</v>
@@ -3432,7 +3432,7 @@
         <v>108.9</v>
       </c>
       <c r="D172" s="4">
-        <v>100.79179999999999</v>
+        <v>100.75830000000001</v>
       </c>
       <c r="E172" s="4">
         <v>234.78100000000001</v>
@@ -3449,7 +3449,7 @@
         <v>107.48</v>
       </c>
       <c r="D173" s="4">
-        <v>101.7782</v>
+        <v>101.77670000000001</v>
       </c>
       <c r="E173" s="4">
         <v>236.29300000000001</v>
@@ -3466,7 +3466,7 @@
         <v>107.76</v>
       </c>
       <c r="D174" s="4">
-        <v>101.83369999999999</v>
+        <v>101.8425</v>
       </c>
       <c r="E174" s="4">
         <v>237.072</v>
@@ -3483,7 +3483,7 @@
         <v>109.54</v>
       </c>
       <c r="D175" s="4">
-        <v>102.2325</v>
+        <v>102.2594</v>
       </c>
       <c r="E175" s="4">
         <v>237.9</v>
@@ -3500,7 +3500,7 @@
         <v>111.8</v>
       </c>
       <c r="D176" s="4">
-        <v>102.5722</v>
+        <v>102.5986</v>
       </c>
       <c r="E176" s="4">
         <v>238.34299999999999</v>
@@ -3517,7 +3517,7 @@
         <v>106.77</v>
       </c>
       <c r="D177" s="4">
-        <v>102.8479</v>
+        <v>102.8163</v>
       </c>
       <c r="E177" s="4">
         <v>238.25</v>
@@ -3534,7 +3534,7 @@
         <v>101.61</v>
       </c>
       <c r="D178" s="4">
-        <v>102.6491</v>
+        <v>102.6562</v>
       </c>
       <c r="E178" s="4">
         <v>237.852</v>
@@ -3551,7 +3551,7 @@
         <v>97.09</v>
       </c>
       <c r="D179" s="4">
-        <v>102.9858</v>
+        <v>102.9776</v>
       </c>
       <c r="E179" s="4">
         <v>238.03100000000001</v>
@@ -3568,7 +3568,7 @@
         <v>87.43</v>
       </c>
       <c r="D180" s="4">
-        <v>102.9911</v>
+        <v>102.9892</v>
       </c>
       <c r="E180" s="4">
         <v>237.43299999999999</v>
@@ -3585,7 +3585,7 @@
         <v>79.44</v>
       </c>
       <c r="D181" s="4">
-        <v>103.6669</v>
+        <v>103.64019999999999</v>
       </c>
       <c r="E181" s="4">
         <v>236.15100000000001</v>
@@ -3602,7 +3602,7 @@
         <v>62.34</v>
       </c>
       <c r="D182" s="4">
-        <v>103.6139</v>
+        <v>103.6345</v>
       </c>
       <c r="E182" s="4">
         <v>234.81200000000001</v>
@@ -3619,7 +3619,7 @@
         <v>47.76</v>
       </c>
       <c r="D183" s="4">
-        <v>102.8479</v>
+        <v>102.82389999999999</v>
       </c>
       <c r="E183" s="4">
         <v>233.70699999999999</v>
@@ -3636,7 +3636,7 @@
         <v>58.1</v>
       </c>
       <c r="D184" s="4">
-        <v>102.22920000000001</v>
+        <v>102.15130000000001</v>
       </c>
       <c r="E184" s="4">
         <v>234.72200000000001</v>
@@ -3653,7 +3653,7 @@
         <v>55.89</v>
       </c>
       <c r="D185" s="4">
-        <v>101.89449999999999</v>
+        <v>101.824</v>
       </c>
       <c r="E185" s="4">
         <v>236.119</v>
@@ -3670,7 +3670,7 @@
         <v>59.52</v>
       </c>
       <c r="D186" s="4">
-        <v>101.2859</v>
+        <v>101.244</v>
       </c>
       <c r="E186" s="4">
         <v>236.59899999999999</v>
@@ -3687,7 +3687,7 @@
         <v>64.08</v>
       </c>
       <c r="D187" s="4">
-        <v>100.8408</v>
+        <v>100.783</v>
       </c>
       <c r="E187" s="4">
         <v>237.80500000000001</v>
@@ -3704,7 +3704,7 @@
         <v>61.48</v>
       </c>
       <c r="D188" s="4">
-        <v>100.5063</v>
+        <v>100.4781</v>
       </c>
       <c r="E188" s="4">
         <v>238.63800000000001</v>
@@ -3721,7 +3721,7 @@
         <v>56.56</v>
       </c>
       <c r="D189" s="4">
-        <v>101.1831</v>
+        <v>101.1052</v>
       </c>
       <c r="E189" s="4">
         <v>238.654</v>
@@ -3738,7 +3738,7 @@
         <v>46.52</v>
       </c>
       <c r="D190" s="4">
-        <v>100.9115</v>
+        <v>100.9442</v>
       </c>
       <c r="E190" s="4">
         <v>238.316</v>
@@ -3755,7 +3755,7 @@
         <v>47.62</v>
       </c>
       <c r="D191" s="4">
-        <v>100.568</v>
+        <v>100.6507</v>
       </c>
       <c r="E191" s="4">
         <v>237.94499999999999</v>
@@ -3772,7 +3772,7 @@
         <v>48.43</v>
       </c>
       <c r="D192" s="4">
-        <v>100.1588</v>
+        <v>100.1871</v>
       </c>
       <c r="E192" s="4">
         <v>237.83799999999999</v>
@@ -3789,7 +3789,7 @@
         <v>44.27</v>
       </c>
       <c r="D193" s="4">
-        <v>99.409899999999993</v>
+        <v>99.438199999999995</v>
       </c>
       <c r="E193" s="4">
         <v>237.33600000000001</v>
@@ -3806,7 +3806,7 @@
         <v>38.01</v>
       </c>
       <c r="D194" s="4">
-        <v>98.832899999999995</v>
+        <v>98.938999999999993</v>
       </c>
       <c r="E194" s="4">
         <v>236.52500000000001</v>
@@ -3823,7 +3823,7 @@
         <v>30.7</v>
       </c>
       <c r="D195" s="4">
-        <v>99.479699999999994</v>
+        <v>99.455799999999996</v>
       </c>
       <c r="E195" s="4">
         <v>236.916</v>
@@ -3840,7 +3840,7 @@
         <v>32.18</v>
       </c>
       <c r="D196" s="4">
-        <v>98.958299999999994</v>
+        <v>98.913600000000002</v>
       </c>
       <c r="E196" s="4">
         <v>237.11099999999999</v>
@@ -3857,7 +3857,7 @@
         <v>38.21</v>
       </c>
       <c r="D197" s="4">
-        <v>98.195400000000006</v>
+        <v>98.190700000000007</v>
       </c>
       <c r="E197" s="4">
         <v>238.13200000000001</v>
@@ -3874,7 +3874,7 @@
         <v>41.58</v>
       </c>
       <c r="D198" s="4">
-        <v>98.467299999999994</v>
+        <v>98.466899999999995</v>
       </c>
       <c r="E198" s="4">
         <v>239.261</v>
@@ -3891,7 +3891,7 @@
         <v>46.74</v>
       </c>
       <c r="D199" s="4">
-        <v>98.288899999999998</v>
+        <v>98.251800000000003</v>
       </c>
       <c r="E199" s="4">
         <v>240.22900000000001</v>
@@ -3908,7 +3908,7 @@
         <v>48.25</v>
       </c>
       <c r="D200" s="4">
-        <v>98.720100000000002</v>
+        <v>98.727500000000006</v>
       </c>
       <c r="E200" s="4">
         <v>241.018</v>
@@ -3925,7 +3925,7 @@
         <v>44.95</v>
       </c>
       <c r="D201" s="4">
-        <v>98.899199999999993</v>
+        <v>98.835999999999999</v>
       </c>
       <c r="E201" s="4">
         <v>240.62799999999999</v>
@@ -3942,7 +3942,7 @@
         <v>45.84</v>
       </c>
       <c r="D202" s="4">
-        <v>98.724900000000005</v>
+        <v>98.755399999999995</v>
       </c>
       <c r="E202" s="4">
         <v>240.84899999999999</v>
@@ -3959,7 +3959,7 @@
         <v>46.57</v>
       </c>
       <c r="D203" s="4">
-        <v>98.605999999999995</v>
+        <v>98.659599999999998</v>
       </c>
       <c r="E203" s="4">
         <v>241.428</v>
@@ -3976,7 +3976,7 @@
         <v>49.52</v>
       </c>
       <c r="D204" s="4">
-        <v>98.670299999999997</v>
+        <v>98.732200000000006</v>
       </c>
       <c r="E204" s="4">
         <v>241.72900000000001</v>
@@ -3993,7 +3993,7 @@
         <v>44.73</v>
       </c>
       <c r="D205" s="4">
-        <v>98.228800000000007</v>
+        <v>98.345200000000006</v>
       </c>
       <c r="E205" s="4">
         <v>241.35300000000001</v>
@@ -4010,7 +4010,7 @@
         <v>53.31</v>
       </c>
       <c r="D206" s="4">
-        <v>98.895799999999994</v>
+        <v>99.031400000000005</v>
       </c>
       <c r="E206" s="4">
         <v>241.43199999999999</v>
@@ -4027,7 +4027,7 @@
         <v>54.58</v>
       </c>
       <c r="D207" s="4">
-        <v>98.744600000000005</v>
+        <v>98.798699999999997</v>
       </c>
       <c r="E207" s="4">
         <v>242.839</v>
@@ -4044,7 +4044,7 @@
         <v>54.87</v>
       </c>
       <c r="D208" s="4">
-        <v>98.367599999999996</v>
+        <v>98.432199999999995</v>
       </c>
       <c r="E208" s="4">
         <v>243.60300000000001</v>
@@ -4061,7 +4061,7 @@
         <v>51.59</v>
       </c>
       <c r="D209" s="4">
-        <v>99.106499999999997</v>
+        <v>99.066299999999998</v>
       </c>
       <c r="E209" s="4">
         <v>243.80099999999999</v>
@@ -4078,7 +4078,7 @@
         <v>52.31</v>
       </c>
       <c r="D210" s="4">
-        <v>100.0363</v>
+        <v>100.0082</v>
       </c>
       <c r="E210" s="4">
         <v>244.524</v>
@@ -4095,7 +4095,7 @@
         <v>50.33</v>
       </c>
       <c r="D211" s="4">
-        <v>100.14700000000001</v>
+        <v>100.12860000000001</v>
       </c>
       <c r="E211" s="4">
         <v>244.733</v>
@@ -4112,7 +4112,7 @@
         <v>46.37</v>
       </c>
       <c r="D212" s="4">
-        <v>100.30419999999999</v>
+        <v>100.3233</v>
       </c>
       <c r="E212" s="4">
         <v>244.95500000000001</v>
@@ -4129,7 +4129,7 @@
         <v>48.48</v>
       </c>
       <c r="D213" s="4">
-        <v>100.2092</v>
+        <v>100.0947</v>
       </c>
       <c r="E213" s="4">
         <v>244.786</v>
@@ -4146,7 +4146,7 @@
         <v>51.7</v>
       </c>
       <c r="D214" s="4">
-        <v>99.705500000000001</v>
+        <v>99.664199999999994</v>
       </c>
       <c r="E214" s="4">
         <v>245.51900000000001</v>
@@ -4163,7 +4163,7 @@
         <v>56.15</v>
       </c>
       <c r="D215" s="4">
-        <v>99.748500000000007</v>
+        <v>99.768600000000006</v>
       </c>
       <c r="E215" s="4">
         <v>246.81899999999999</v>
@@ -4180,7 +4180,7 @@
         <v>57.51</v>
       </c>
       <c r="D216" s="4">
-        <v>100.988</v>
+        <v>100.99809999999999</v>
       </c>
       <c r="E216" s="4">
         <v>246.66300000000001</v>
@@ -4197,7 +4197,7 @@
         <v>62.71</v>
       </c>
       <c r="D217" s="4">
-        <v>101.273</v>
+        <v>101.2597</v>
       </c>
       <c r="E217" s="4">
         <v>246.66900000000001</v>
@@ -4214,7 +4214,7 @@
         <v>64.37</v>
       </c>
       <c r="D218" s="4">
-        <v>101.36960000000001</v>
+        <v>101.4573</v>
       </c>
       <c r="E218" s="4">
         <v>246.524</v>
@@ -4231,7 +4231,7 @@
         <v>69.08</v>
       </c>
       <c r="D219" s="4">
-        <v>101.3561</v>
+        <v>101.3939</v>
       </c>
       <c r="E219" s="4">
         <v>247.86699999999999</v>
@@ -4248,7 +4248,7 @@
         <v>65.319999999999993</v>
       </c>
       <c r="D220" s="4">
-        <v>101.6495</v>
+        <v>101.76560000000001</v>
       </c>
       <c r="E220" s="4">
         <v>248.99100000000001</v>
@@ -4265,7 +4265,7 @@
         <v>66.02</v>
       </c>
       <c r="D221" s="4">
-        <v>102.298</v>
+        <v>102.2441</v>
       </c>
       <c r="E221" s="4">
         <v>249.554</v>
@@ -4282,7 +4282,7 @@
         <v>72.11</v>
       </c>
       <c r="D222" s="4">
-        <v>103.40949999999999</v>
+        <v>103.3468</v>
       </c>
       <c r="E222" s="4">
         <v>250.54599999999999</v>
@@ -4299,7 +4299,7 @@
         <v>76.98</v>
       </c>
       <c r="D223" s="4">
-        <v>102.5408</v>
+        <v>102.39109999999999</v>
       </c>
       <c r="E223" s="4">
         <v>251.58799999999999</v>
@@ -4316,7 +4316,7 @@
         <v>74.41</v>
       </c>
       <c r="D224" s="4">
-        <v>103.3045</v>
+        <v>103.19240000000001</v>
       </c>
       <c r="E224" s="4">
         <v>251.989</v>
@@ -4333,7 +4333,7 @@
         <v>74.25</v>
       </c>
       <c r="D225" s="4">
-        <v>103.5474</v>
+        <v>103.3334</v>
       </c>
       <c r="E225" s="4">
         <v>252.006</v>
@@ -4350,7 +4350,7 @@
         <v>72.53</v>
       </c>
       <c r="D226" s="4">
-        <v>104.16589999999999</v>
+        <v>104.08069999999999</v>
       </c>
       <c r="E226" s="4">
         <v>252.14599999999999</v>
@@ -4367,7 +4367,7 @@
         <v>78.89</v>
       </c>
       <c r="D227" s="4">
-        <v>104.1315</v>
+        <v>104.1181</v>
       </c>
       <c r="E227" s="4">
         <v>252.43899999999999</v>
@@ -4384,7 +4384,7 @@
         <v>81.03</v>
       </c>
       <c r="D228" s="4">
-        <v>103.98739999999999</v>
+        <v>103.9397</v>
       </c>
       <c r="E228" s="4">
         <v>252.88499999999999</v>
@@ -4401,7 +4401,7 @@
         <v>64.75</v>
       </c>
       <c r="D229" s="4">
-        <v>103.9127</v>
+        <v>104.00069999999999</v>
       </c>
       <c r="E229" s="4">
         <v>252.03800000000001</v>
@@ -4418,7 +4418,7 @@
         <v>57.36</v>
       </c>
       <c r="D230" s="4">
-        <v>103.867</v>
+        <v>103.99460000000001</v>
       </c>
       <c r="E230" s="4">
         <v>251.233</v>
@@ -4435,7 +4435,7 @@
         <v>59.41</v>
       </c>
       <c r="D231" s="4">
-        <v>103.3023</v>
+        <v>103.373</v>
       </c>
       <c r="E231" s="4">
         <v>251.71199999999999</v>
@@ -4452,7 +4452,7 @@
         <v>63.96</v>
       </c>
       <c r="D232" s="4">
-        <v>102.72799999999999</v>
+        <v>102.8292</v>
       </c>
       <c r="E232" s="4">
         <v>252.77600000000001</v>
@@ -4469,7 +4469,7 @@
         <v>66.14</v>
       </c>
       <c r="D233" s="4">
-        <v>102.8635</v>
+        <v>102.82859999999999</v>
       </c>
       <c r="E233" s="4">
         <v>254.202</v>
@@ -4486,7 +4486,7 @@
         <v>71.23</v>
       </c>
       <c r="D234" s="4">
-        <v>102.2543</v>
+        <v>102.24809999999999</v>
       </c>
       <c r="E234" s="4">
         <v>255.548</v>
@@ -4503,7 +4503,7 @@
         <v>71.319999999999993</v>
       </c>
       <c r="D235" s="4">
-        <v>102.45189999999999</v>
+        <v>102.4192</v>
       </c>
       <c r="E235" s="4">
         <v>256.09199999999998</v>
@@ -4520,7 +4520,7 @@
         <v>64.22</v>
       </c>
       <c r="D236" s="4">
-        <v>102.384</v>
+        <v>102.4893</v>
       </c>
       <c r="E236" s="4">
         <v>256.14299999999997</v>
@@ -4537,7 +4537,7 @@
         <v>63.92</v>
       </c>
       <c r="D237" s="4">
-        <v>102.0568</v>
+        <v>102.0236</v>
       </c>
       <c r="E237" s="4">
         <v>256.57100000000003</v>
@@ -4554,7 +4554,7 @@
         <v>59.04</v>
       </c>
       <c r="D238" s="4">
-        <v>102.68819999999999</v>
+        <v>102.7754</v>
       </c>
       <c r="E238" s="4">
         <v>256.55799999999999</v>
@@ -4571,7 +4571,7 @@
         <v>62.83</v>
       </c>
       <c r="D239" s="4">
-        <v>102.3143</v>
+        <v>102.53149999999999</v>
       </c>
       <c r="E239" s="4">
         <v>256.75900000000001</v>
@@ -4588,7 +4588,7 @@
         <v>59.71</v>
       </c>
       <c r="D240" s="4">
-        <v>101.4645</v>
+        <v>101.6022</v>
       </c>
       <c r="E240" s="4">
         <v>257.346</v>
@@ -4605,7 +4605,7 @@
         <v>63.21</v>
       </c>
       <c r="D241" s="4">
-        <v>101.9876</v>
+        <v>102.148</v>
       </c>
       <c r="E241" s="4">
         <v>257.20800000000003</v>
@@ -4622,7 +4622,7 @@
         <v>67.31</v>
       </c>
       <c r="D242" s="4">
-        <v>101.61790000000001</v>
+        <v>101.884</v>
       </c>
       <c r="E242" s="4">
         <v>256.97399999999999</v>
@@ -4639,7 +4639,7 @@
         <v>63.65</v>
       </c>
       <c r="D243" s="4">
-        <v>101.09180000000001</v>
+        <v>101.3768</v>
       </c>
       <c r="E243" s="4">
         <v>257.971</v>
@@ -4656,7 +4656,7 @@
         <v>55.66</v>
       </c>
       <c r="D244" s="4">
-        <v>101.32470000000001</v>
+        <v>101.633</v>
       </c>
       <c r="E244" s="4">
         <v>258.678</v>
@@ -4673,7 +4673,7 @@
         <v>32.01</v>
       </c>
       <c r="D245" s="4">
-        <v>97.447699999999998</v>
+        <v>97.667199999999994</v>
       </c>
       <c r="E245" s="4">
         <v>258.11500000000001</v>
@@ -4690,7 +4690,7 @@
         <v>18.38</v>
       </c>
       <c r="D246" s="4">
-        <v>84.201800000000006</v>
+        <v>84.597899999999996</v>
       </c>
       <c r="E246" s="4">
         <v>256.38900000000001</v>
@@ -4707,7 +4707,7 @@
         <v>29.38</v>
       </c>
       <c r="D247" s="4">
-        <v>85.843400000000003</v>
+        <v>85.973200000000006</v>
       </c>
       <c r="E247" s="4">
         <v>256.39400000000001</v>
@@ -4724,7 +4724,7 @@
         <v>40.270000000000003</v>
       </c>
       <c r="D248" s="4">
-        <v>91.162199999999999</v>
+        <v>91.5625</v>
       </c>
       <c r="E248" s="4">
         <v>257.79700000000003</v>
@@ -4741,7 +4741,7 @@
         <v>43.24</v>
       </c>
       <c r="D249" s="4">
-        <v>94.8887</v>
+        <v>95.014399999999995</v>
       </c>
       <c r="E249" s="4">
         <v>259.101</v>
@@ -4758,7 +4758,7 @@
         <v>44.74</v>
       </c>
       <c r="D250" s="4">
-        <v>95.892399999999995</v>
+        <v>95.888099999999994</v>
       </c>
       <c r="E250" s="4">
         <v>259.91800000000001</v>
@@ -4775,7 +4775,7 @@
         <v>40.909999999999997</v>
       </c>
       <c r="D251" s="4">
-        <v>95.601900000000001</v>
+        <v>95.844399999999993</v>
       </c>
       <c r="E251" s="4">
         <v>260.27999999999997</v>
@@ -4792,7 +4792,7 @@
         <v>40.19</v>
       </c>
       <c r="D252" s="4">
-        <v>96.645399999999995</v>
+        <v>96.429199999999994</v>
       </c>
       <c r="E252" s="4">
         <v>260.38799999999998</v>
@@ -4809,7 +4809,7 @@
         <v>42.69</v>
       </c>
       <c r="D253" s="4">
-        <v>97.160899999999998</v>
+        <v>96.856399999999994</v>
       </c>
       <c r="E253" s="4">
         <v>260.22899999999998</v>
@@ -4826,7 +4826,7 @@
         <v>49.99</v>
       </c>
       <c r="D254" s="4">
-        <v>98.285399999999996</v>
+        <v>97.975399999999993</v>
       </c>
       <c r="E254" s="4">
         <v>260.47399999999999</v>
@@ -4843,7 +4843,7 @@
         <v>54.77</v>
       </c>
       <c r="D255" s="4">
-        <v>99.407600000000002</v>
+        <v>98.783600000000007</v>
       </c>
       <c r="E255" s="4">
         <v>261.58199999999999</v>
@@ -4860,7 +4860,7 @@
         <v>62.28</v>
       </c>
       <c r="D256" s="4">
-        <v>96.396600000000007</v>
+        <v>95.374399999999994</v>
       </c>
       <c r="E256" s="4">
         <v>263.01400000000001</v>
@@ -4877,7 +4877,7 @@
         <v>65.41</v>
       </c>
       <c r="D257" s="4">
-        <v>99.161799999999999</v>
+        <v>98.135099999999994</v>
       </c>
       <c r="E257" s="4">
         <v>264.87700000000001</v>
@@ -4894,7 +4894,7 @@
         <v>64.81</v>
       </c>
       <c r="D258" s="4">
-        <v>99.241600000000005</v>
+        <v>98.288600000000002</v>
       </c>
       <c r="E258" s="4">
         <v>267.05399999999997</v>
@@ -4911,7 +4911,7 @@
         <v>68.53</v>
       </c>
       <c r="D259" s="5">
-        <v>99.922600000000003</v>
+        <v>99.150800000000004</v>
       </c>
       <c r="E259" s="5">
         <v>269.19499999999999</v>
@@ -4928,7 +4928,7 @@
         <v>73.16</v>
       </c>
       <c r="D260" s="5">
-        <v>100.4704</v>
+        <v>99.509600000000006</v>
       </c>
       <c r="E260" s="5">
         <v>271.69600000000003</v>
@@ -4945,7 +4945,7 @@
         <v>75.17</v>
       </c>
       <c r="D261" s="5">
-        <v>101.16759999999999</v>
+        <v>100.12309999999999</v>
       </c>
       <c r="E261" s="5">
         <v>273.00299999999999</v>
@@ -4962,7 +4962,7 @@
         <v>70.75</v>
       </c>
       <c r="D262" s="5">
-        <v>101.09269999999999</v>
+        <v>100.1255</v>
       </c>
       <c r="E262" s="5">
         <v>273.56700000000001</v>
@@ -4979,7 +4979,7 @@
         <v>74.489999999999995</v>
       </c>
       <c r="D263" s="5">
-        <v>99.860600000000005</v>
+        <v>99.061400000000006</v>
       </c>
       <c r="E263" s="5">
         <v>274.31</v>
@@ -4996,7 +4996,7 @@
         <v>83.54</v>
       </c>
       <c r="D264" s="5">
-        <v>101.2534</v>
+        <v>100.3045</v>
       </c>
       <c r="E264" s="5">
         <v>276.589</v>
@@ -5013,7 +5013,7 @@
         <v>81.05</v>
       </c>
       <c r="D265" s="5">
-        <v>101.99769999999999</v>
+        <v>101.19710000000001</v>
       </c>
       <c r="E265" s="5">
         <v>277.94799999999998</v>
@@ -5030,7 +5030,7 @@
         <v>74.17</v>
       </c>
       <c r="D266" s="5">
-        <v>101.7015</v>
+        <v>100.886</v>
       </c>
       <c r="E266" s="5">
         <v>278.80200000000002</v>
@@ -5047,7 +5047,7 @@
         <v>86.51</v>
       </c>
       <c r="D267" s="5">
-        <v>102.5596</v>
+        <v>101.0227</v>
       </c>
       <c r="E267" s="5">
         <v>281.14800000000002</v>
@@ -5064,7 +5064,7 @@
         <v>97.13</v>
       </c>
       <c r="D268" s="5">
-        <v>103.58450000000001</v>
+        <v>101.67659999999999</v>
       </c>
       <c r="E268" s="5">
         <v>283.71600000000001</v>
@@ -5081,7 +5081,7 @@
         <v>117.25</v>
       </c>
       <c r="D269" s="5">
-        <v>104.47410000000001</v>
+        <v>102.47799999999999</v>
       </c>
       <c r="E269" s="5">
         <v>287.50400000000002</v>
@@ -5098,7 +5098,7 @@
         <v>104.58</v>
       </c>
       <c r="D270" s="5">
-        <v>105.5973</v>
+        <v>102.7953</v>
       </c>
       <c r="E270" s="5">
         <v>289.10899999999998</v>
@@ -5115,7 +5115,7 @@
         <v>113.34</v>
       </c>
       <c r="D271" s="5">
-        <v>106.12939999999999</v>
+        <v>102.7769</v>
       </c>
       <c r="E271" s="5">
         <v>292.29599999999999</v>
@@ -5129,13 +5129,13 @@
         <v>119.31</v>
       </c>
       <c r="C272" s="5">
-        <v>122.7</v>
+        <v>122.71</v>
       </c>
       <c r="D272" s="5">
-        <v>104.1</v>
+        <v>102.6863</v>
       </c>
       <c r="E272" s="5">
-        <v>296.3</v>
+        <v>296.31099999999998</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -5146,13 +5146,13 @@
         <v>120.27</v>
       </c>
       <c r="C273" s="5">
-        <v>111.9</v>
+        <v>111.93</v>
       </c>
       <c r="D273" s="5">
-        <v>104.8</v>
+        <v>103.1328</v>
       </c>
       <c r="E273" s="5">
-        <v>296.3</v>
+        <v>296.27600000000001</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
@@ -5163,13 +5163,13 @@
         <v>121.5</v>
       </c>
       <c r="C274" s="5">
-        <v>100.5</v>
+        <v>100.45</v>
       </c>
       <c r="D274" s="5">
-        <v>104.7</v>
+        <v>103.23439999999999</v>
       </c>
       <c r="E274" s="5">
-        <v>296.2</v>
+        <v>296.17099999999999</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -5180,13 +5180,13 @@
         <v>122.63</v>
       </c>
       <c r="C275" s="5">
-        <v>89.8</v>
+        <v>89.76</v>
       </c>
       <c r="D275" s="5">
-        <v>104.8</v>
+        <v>103.5283</v>
       </c>
       <c r="E275" s="5">
-        <v>296.8</v>
+        <v>296.80799999999999</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
@@ -5197,34 +5197,133 @@
         <v>123.51</v>
       </c>
       <c r="C276" s="5">
-        <v>93.3</v>
+        <v>93.33</v>
       </c>
       <c r="D276" s="5">
-        <v>104.7</v>
+        <v>103.4114</v>
       </c>
       <c r="E276" s="5">
-        <v>298</v>
+        <v>298.012</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C277" s="5"/>
-      <c r="D277" s="5"/>
-      <c r="E277" s="5"/>
+      <c r="A277" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B277" s="5">
+        <v>124.46</v>
+      </c>
+      <c r="C277" s="5">
+        <v>91.42</v>
+      </c>
+      <c r="D277" s="5">
+        <v>103.0707</v>
+      </c>
+      <c r="E277" s="5">
+        <v>297.71100000000001</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A278" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B278" s="5">
+        <v>126.03</v>
+      </c>
+      <c r="C278" s="5">
+        <v>80.92</v>
+      </c>
+      <c r="D278" s="5">
+        <v>101.48480000000001</v>
+      </c>
+      <c r="E278" s="5">
+        <v>296.79700000000003</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A279" s="1">
+        <v>44927</v>
+      </c>
+      <c r="B279" s="5">
+        <v>128.27000000000001</v>
+      </c>
+      <c r="C279" s="5">
+        <v>82.5</v>
+      </c>
+      <c r="D279" s="5">
+        <v>102.508</v>
+      </c>
+      <c r="E279" s="5">
+        <v>299.17</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A280" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B280" s="5">
+        <v>130.4</v>
+      </c>
+      <c r="C280" s="5">
+        <v>82.59</v>
+      </c>
+      <c r="D280" s="5">
+        <v>102.50230000000001</v>
+      </c>
+      <c r="E280" s="5">
+        <v>300.83999999999997</v>
+      </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C281" s="5"/>
-      <c r="D281" s="5"/>
-      <c r="E281" s="5"/>
+      <c r="A281" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B281" s="5">
+        <v>131.77000000000001</v>
+      </c>
+      <c r="C281" s="5">
+        <v>78.430000000000007</v>
+      </c>
+      <c r="D281" s="5">
+        <v>102.6521</v>
+      </c>
+      <c r="E281" s="5">
+        <v>301.83600000000001</v>
+      </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C282" s="5"/>
-      <c r="D282" s="5"/>
-      <c r="E282" s="5"/>
+      <c r="A282" s="1">
+        <v>45017</v>
+      </c>
+      <c r="B282" s="5">
+        <v>132.80000000000001</v>
+      </c>
+      <c r="C282" s="5">
+        <v>84.64</v>
+      </c>
+      <c r="D282" s="5">
+        <v>103.1748</v>
+      </c>
+      <c r="E282" s="5">
+        <v>303.363</v>
+      </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C283" s="5"/>
-      <c r="D283" s="5"/>
-      <c r="E283" s="5"/>
+      <c r="A283" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B283" s="5">
+        <v>133.38</v>
+      </c>
+      <c r="C283" s="5">
+        <v>75.47</v>
+      </c>
+      <c r="D283" s="5">
+        <v>103.0107</v>
+      </c>
+      <c r="E283" s="5">
+        <v>304.12700000000001</v>
+      </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C284" s="5"/>
@@ -5278,13 +5377,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C921DE1D-2686-44DF-B218-59946BA2C5A6}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:B17"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5316,198 +5415,268 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44866</v>
+        <v>45078</v>
       </c>
       <c r="B4" s="7">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C4" s="8">
-        <v>105.28570000000001</v>
+        <v>104.48977099869612</v>
       </c>
       <c r="D4" s="8">
-        <v>299.55200000000002</v>
+        <v>305.33319983849509</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44896</v>
+        <v>45108</v>
       </c>
       <c r="B5" s="7">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C5" s="8">
-        <v>105.12909999999999</v>
+        <v>104.20712190955291</v>
       </c>
       <c r="D5" s="8">
-        <v>300.49369999999999</v>
+        <v>305.6841316127456</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44927</v>
+        <v>45139</v>
       </c>
       <c r="B6" s="7">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C6" s="8">
-        <v>104.63590000000001</v>
+        <v>104.37592757594578</v>
       </c>
       <c r="D6" s="8">
-        <v>301.19729999999998</v>
+        <v>305.35679390965731</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44958</v>
+        <v>45170</v>
       </c>
       <c r="B7" s="7">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C7" s="8">
-        <v>104.3762</v>
+        <v>104.73848382528293</v>
       </c>
       <c r="D7" s="8">
-        <v>301.95159999999998</v>
+        <v>305.30900454375308</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44986</v>
+        <v>45200</v>
       </c>
       <c r="B8" s="7">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C8" s="8">
-        <v>104.14279999999999</v>
+        <v>104.00299084141793</v>
       </c>
       <c r="D8" s="8">
-        <v>302.65159999999997</v>
+        <v>305.73044749468932</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45017</v>
+        <v>45231</v>
       </c>
       <c r="B9" s="7">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C9" s="8">
-        <v>103.82980000000001</v>
+        <v>103.73689475981928</v>
       </c>
       <c r="D9" s="8">
-        <v>303.20440000000002</v>
+        <v>305.41574448824178</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>45047</v>
+        <v>45261</v>
       </c>
       <c r="B10" s="7">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C10" s="8">
-        <v>103.7283</v>
+        <v>102.22884117763263</v>
       </c>
       <c r="D10" s="8">
-        <v>303.8655</v>
+        <v>304.70596156326303</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45078</v>
+        <v>45292</v>
       </c>
       <c r="B11" s="7">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C11" s="8">
-        <v>103.7323</v>
+        <v>103.10398457828218</v>
       </c>
       <c r="D11" s="8">
-        <v>304.54219999999998</v>
+        <v>306.30412582519239</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>45108</v>
+        <v>45323</v>
       </c>
       <c r="B12" s="7">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C12" s="8">
-        <v>103.9573</v>
+        <v>103.20097723276452</v>
       </c>
       <c r="D12" s="8">
-        <v>305.19690000000003</v>
+        <v>307.45283915026783</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>45139</v>
+        <v>45352</v>
       </c>
       <c r="B13" s="7">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C13" s="8">
-        <v>104.08620000000001</v>
+        <v>103.45589168866307</v>
       </c>
       <c r="D13" s="8">
-        <v>305.9325</v>
+        <v>308.81654755473681</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45170</v>
+        <v>45383</v>
       </c>
       <c r="B14" s="7">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C14" s="8">
-        <v>104.2342</v>
+        <v>104.10682600156652</v>
       </c>
       <c r="D14" s="8">
-        <v>306.71159999999998</v>
+        <v>309.54146312269324</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>45200</v>
+        <v>45413</v>
       </c>
       <c r="B15" s="7">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C15" s="8">
-        <v>104.4456</v>
+        <v>104.02858992715471</v>
       </c>
       <c r="D15" s="8">
-        <v>307.6277</v>
+        <v>310.51352669156574</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>45231</v>
+        <v>45444</v>
       </c>
       <c r="B16" s="7">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C16" s="8">
-        <v>104.59869999999999</v>
+        <v>105.59450466389725</v>
       </c>
       <c r="D16" s="8">
-        <v>308.42380000000003</v>
+        <v>311.76124074638301</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45261</v>
+        <v>45474</v>
       </c>
       <c r="B17" s="7">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C17" s="8">
-        <v>104.73779999999999</v>
+        <v>105.34023898820938</v>
       </c>
       <c r="D17" s="8">
-        <v>309.19330000000002</v>
+        <v>312.47027874879512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45505</v>
+      </c>
+      <c r="B18" s="7">
+        <v>84</v>
+      </c>
+      <c r="C18" s="8">
+        <v>105.56884414881465</v>
+      </c>
+      <c r="D18" s="8">
+        <v>312.18240621495329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45536</v>
+      </c>
+      <c r="B19" s="7">
+        <v>84</v>
+      </c>
+      <c r="C19" s="8">
+        <v>105.99571174190262</v>
+      </c>
+      <c r="D19" s="8">
+        <v>312.10916759819111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45566</v>
+      </c>
+      <c r="B20" s="7">
+        <v>85</v>
+      </c>
+      <c r="C20" s="8">
+        <v>105.33164794989874</v>
+      </c>
+      <c r="D20" s="8">
+        <v>312.45671175588194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B21" s="7">
+        <v>85</v>
+      </c>
+      <c r="C21" s="8">
+        <v>105.11214169058714</v>
+      </c>
+      <c r="D21" s="8">
+        <v>311.96054491322786</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B22" s="7">
+        <v>85</v>
+      </c>
+      <c r="C22" s="8">
+        <v>103.62174676337028</v>
+      </c>
+      <c r="D22" s="8">
+        <v>310.98268356299548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion base y programa
</commit_message>
<xml_diff>
--- a/Base_Modelo_ARIMAX.xlsx
+++ b/Base_Modelo_ARIMAX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\repos\ARIMAX_Conditional_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B91C9-5327-4560-B881-A88A644F9995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4E9E50-9CDC-4C28-B46D-977BF97AFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -502,11 +502,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88848EC6-D3A9-432A-B99B-25298BB184AA}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B261" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B283" sqref="B283"/>
+      <selection pane="bottomRight" activeCell="B284" sqref="B284:B288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5248,10 +5248,10 @@
         <v>128.27000000000001</v>
       </c>
       <c r="C279" s="5">
-        <v>82.5</v>
+        <v>83.76173913043479</v>
       </c>
       <c r="D279" s="5">
-        <v>102.508</v>
+        <v>102.5478</v>
       </c>
       <c r="E279" s="5">
         <v>299.17</v>
@@ -5265,10 +5265,10 @@
         <v>130.4</v>
       </c>
       <c r="C280" s="5">
-        <v>82.59</v>
+        <v>83.511904761904773</v>
       </c>
       <c r="D280" s="5">
-        <v>102.50230000000001</v>
+        <v>102.5671</v>
       </c>
       <c r="E280" s="5">
         <v>300.83999999999997</v>
@@ -5282,10 +5282,10 @@
         <v>131.77000000000001</v>
       </c>
       <c r="C281" s="5">
-        <v>78.430000000000007</v>
+        <v>79.031250000000014</v>
       </c>
       <c r="D281" s="5">
-        <v>102.6521</v>
+        <v>102.6592</v>
       </c>
       <c r="E281" s="5">
         <v>301.83600000000001</v>
@@ -5299,10 +5299,10 @@
         <v>132.80000000000001</v>
       </c>
       <c r="C282" s="5">
-        <v>84.64</v>
+        <v>83.456500000000005</v>
       </c>
       <c r="D282" s="5">
-        <v>103.1748</v>
+        <v>103.1512</v>
       </c>
       <c r="E282" s="5">
         <v>303.363</v>
@@ -5316,39 +5316,99 @@
         <v>133.38</v>
       </c>
       <c r="C283" s="5">
-        <v>75.47</v>
+        <v>75.694782608695647</v>
       </c>
       <c r="D283" s="5">
-        <v>103.0107</v>
+        <v>102.92400000000001</v>
       </c>
       <c r="E283" s="5">
         <v>304.12700000000001</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C284" s="5"/>
-      <c r="D284" s="5"/>
-      <c r="E284" s="5"/>
+      <c r="A284" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B284" s="5">
+        <v>133.78</v>
+      </c>
+      <c r="C284" s="5">
+        <v>75.049565217391304</v>
+      </c>
+      <c r="D284" s="5">
+        <v>102.303</v>
+      </c>
+      <c r="E284" s="5">
+        <v>305.10899999999998</v>
+      </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C285" s="5"/>
-      <c r="D285" s="5"/>
-      <c r="E285" s="5"/>
+      <c r="A285" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B285" s="5">
+        <v>134.44999999999999</v>
+      </c>
+      <c r="C285" s="5">
+        <v>80.160000000000011</v>
+      </c>
+      <c r="D285" s="5">
+        <v>103.267</v>
+      </c>
+      <c r="E285" s="5">
+        <v>305.69099999999997</v>
+      </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C286" s="5"/>
-      <c r="D286" s="5"/>
-      <c r="E286" s="5"/>
+      <c r="A286" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B286" s="5">
+        <v>135.38999999999999</v>
+      </c>
+      <c r="C286" s="5">
+        <v>85.104347826086936</v>
+      </c>
+      <c r="D286" s="5">
+        <v>103.2927</v>
+      </c>
+      <c r="E286" s="5">
+        <v>307.02600000000001</v>
+      </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C287" s="5"/>
-      <c r="D287" s="5"/>
-      <c r="E287" s="5"/>
+      <c r="A287" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B287" s="5">
+        <v>136.11000000000001</v>
+      </c>
+      <c r="C287" s="5">
+        <v>92.61818181818181</v>
+      </c>
+      <c r="D287" s="5">
+        <v>103.3643</v>
+      </c>
+      <c r="E287" s="5">
+        <v>307.78899999999999</v>
+      </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C288" s="5"/>
-      <c r="D288" s="5"/>
-      <c r="E288" s="5"/>
+      <c r="A288" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B288" s="5">
+        <v>136.44999999999999</v>
+      </c>
+      <c r="C288" s="5">
+        <v>88.704090909090937</v>
+      </c>
+      <c r="D288" s="5">
+        <v>102.7081</v>
+      </c>
+      <c r="E288" s="5">
+        <v>307.67099999999999</v>
+      </c>
     </row>
     <row r="289" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C289" s="5"/>
@@ -5377,13 +5437,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C921DE1D-2686-44DF-B218-59946BA2C5A6}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5415,268 +5475,198 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45078</v>
+        <v>45231</v>
       </c>
       <c r="B4" s="7">
-        <v>77</v>
+        <v>82.03</v>
       </c>
       <c r="C4" s="8">
-        <v>104.48977099869612</v>
+        <v>102.6262</v>
       </c>
       <c r="D4" s="8">
-        <v>305.33319983849509</v>
+        <v>308.04267604203642</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>45108</v>
+        <v>45261</v>
       </c>
       <c r="B5" s="7">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C5" s="8">
-        <v>104.20712190955291</v>
+        <v>102.401</v>
       </c>
       <c r="D5" s="8">
-        <v>305.6841316127456</v>
+        <v>307.94154841131808</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45139</v>
+        <v>45292</v>
       </c>
       <c r="B6" s="7">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C6" s="8">
-        <v>104.37592757594578</v>
+        <v>102.1699</v>
       </c>
       <c r="D6" s="8">
-        <v>305.35679390965731</v>
+        <v>305.72275480275243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45170</v>
+        <v>45323</v>
       </c>
       <c r="B7" s="7">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C7" s="8">
-        <v>104.73848382528293</v>
+        <v>101.9945</v>
       </c>
       <c r="D7" s="8">
-        <v>305.30900454375308</v>
+        <v>307.53957550853977</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>45200</v>
+        <v>45352</v>
       </c>
       <c r="B8" s="7">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C8" s="8">
-        <v>104.00299084141793</v>
+        <v>101.8523</v>
       </c>
       <c r="D8" s="8">
-        <v>305.73044749468932</v>
+        <v>309.62094592588664</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45231</v>
+        <v>45383</v>
       </c>
       <c r="B9" s="7">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C9" s="8">
-        <v>103.73689475981928</v>
+        <v>101.7414</v>
       </c>
       <c r="D9" s="8">
-        <v>305.41574448824178</v>
+        <v>310.08014697442871</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>45261</v>
+        <v>45413</v>
       </c>
       <c r="B10" s="7">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C10" s="8">
-        <v>102.22884117763263</v>
+        <v>101.74064689673681</v>
       </c>
       <c r="D10" s="8">
-        <v>304.70596156326303</v>
+        <v>311.80862095887159</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45292</v>
+        <v>45444</v>
       </c>
       <c r="B11" s="7">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C11" s="8">
-        <v>103.10398457828218</v>
+        <v>101.63853115187442</v>
       </c>
       <c r="D11" s="8">
-        <v>306.30412582519239</v>
+        <v>312.57544488893865</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>45323</v>
+        <v>45474</v>
       </c>
       <c r="B12" s="7">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C12" s="8">
-        <v>103.20097723276452</v>
+        <v>101.61705949201031</v>
       </c>
       <c r="D12" s="8">
-        <v>307.45283915026783</v>
+        <v>313.60067986811151</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>45352</v>
+        <v>45505</v>
       </c>
       <c r="B13" s="7">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C13" s="8">
-        <v>103.45589168866307</v>
+        <v>101.63379026481607</v>
       </c>
       <c r="D13" s="8">
-        <v>308.81654755473681</v>
+        <v>312.7703144448181</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45383</v>
+        <v>45536</v>
       </c>
       <c r="B14" s="7">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C14" s="8">
-        <v>104.10682600156652</v>
+        <v>101.45666219473706</v>
       </c>
       <c r="D14" s="8">
-        <v>309.54146312269324</v>
+        <v>313.44179205804591</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>45413</v>
+        <v>45566</v>
       </c>
       <c r="B15" s="7">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C15" s="8">
-        <v>104.02858992715471</v>
+        <v>101.62933339229987</v>
       </c>
       <c r="D15" s="8">
-        <v>310.51352669156574</v>
+        <v>314.3195206859703</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>45444</v>
+        <v>45597</v>
       </c>
       <c r="B16" s="7">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C16" s="8">
-        <v>105.59450466389725</v>
+        <v>101.85760000000001</v>
       </c>
       <c r="D16" s="8">
-        <v>311.76124074638301</v>
+        <v>314.00029329100687</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45474</v>
+        <v>45627</v>
       </c>
       <c r="B17" s="7">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C17" s="8">
-        <v>105.34023898820938</v>
+        <v>101.9333</v>
       </c>
       <c r="D17" s="8">
-        <v>312.47027874879512</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>45505</v>
-      </c>
-      <c r="B18" s="7">
-        <v>84</v>
-      </c>
-      <c r="C18" s="8">
-        <v>105.56884414881465</v>
-      </c>
-      <c r="D18" s="8">
-        <v>312.18240621495329</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>45536</v>
-      </c>
-      <c r="B19" s="7">
-        <v>84</v>
-      </c>
-      <c r="C19" s="8">
-        <v>105.99571174190262</v>
-      </c>
-      <c r="D19" s="8">
-        <v>312.10916759819111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>45566</v>
-      </c>
-      <c r="B20" s="7">
-        <v>85</v>
-      </c>
-      <c r="C20" s="8">
-        <v>105.33164794989874</v>
-      </c>
-      <c r="D20" s="8">
-        <v>312.45671175588194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B21" s="7">
-        <v>85</v>
-      </c>
-      <c r="C21" s="8">
-        <v>105.11214169058714</v>
-      </c>
-      <c r="D21" s="8">
-        <v>311.96054491322786</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>45627</v>
-      </c>
-      <c r="B22" s="7">
-        <v>85</v>
-      </c>
-      <c r="C22" s="8">
-        <v>103.62174676337028</v>
-      </c>
-      <c r="D22" s="8">
-        <v>310.98268356299548</v>
+        <v>314.31240770737207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion proyecto y ajustes 250705
</commit_message>
<xml_diff>
--- a/Base_Modelo_ARIMAX.xlsx
+++ b/Base_Modelo_ARIMAX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\repos\ARIMAX_Conditional_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50F04C8-49AD-4558-BDE9-5B964EC131E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54B4A7D-97D2-4F38-86A5-19668700896E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>CPI_EEUU</t>
+  </si>
+  <si>
+    <t>FRED</t>
+  </si>
+  <si>
+    <t>BLS</t>
   </si>
 </sst>
 </file>
@@ -176,9 +182,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -187,6 +190,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,13 +513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88848EC6-D3A9-432A-B99B-25298BB184AA}">
-  <dimension ref="A1:L300"/>
+  <dimension ref="A1:L307"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B289" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C300" sqref="C300:E300"/>
+      <selection pane="bottomRight" activeCell="E323" sqref="E323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5212,7 +5218,7 @@
       <c r="E276" s="4">
         <v>298.012</v>
       </c>
-      <c r="K276" s="10"/>
+      <c r="K276" s="9"/>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
@@ -5230,9 +5236,9 @@
       <c r="E277" s="4">
         <v>297.71100000000001</v>
       </c>
-      <c r="G277" s="8"/>
-      <c r="K277" s="10"/>
-      <c r="L277" s="10"/>
+      <c r="G277" s="7"/>
+      <c r="K277" s="9"/>
+      <c r="L277" s="9"/>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
@@ -5250,9 +5256,9 @@
       <c r="E278" s="4">
         <v>296.79700000000003</v>
       </c>
-      <c r="G278" s="8"/>
-      <c r="K278" s="10"/>
-      <c r="L278" s="10"/>
+      <c r="G278" s="7"/>
+      <c r="K278" s="9"/>
+      <c r="L278" s="9"/>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
@@ -5270,9 +5276,9 @@
       <c r="E279" s="4">
         <v>299.17</v>
       </c>
-      <c r="G279" s="8"/>
-      <c r="K279" s="10"/>
-      <c r="L279" s="10"/>
+      <c r="G279" s="7"/>
+      <c r="K279" s="9"/>
+      <c r="L279" s="9"/>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
@@ -5290,9 +5296,9 @@
       <c r="E280" s="4">
         <v>300.83999999999997</v>
       </c>
-      <c r="G280" s="8"/>
-      <c r="K280" s="10"/>
-      <c r="L280" s="10"/>
+      <c r="G280" s="7"/>
+      <c r="K280" s="9"/>
+      <c r="L280" s="9"/>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
@@ -5310,9 +5316,9 @@
       <c r="E281" s="4">
         <v>301.83600000000001</v>
       </c>
-      <c r="G281" s="8"/>
-      <c r="K281" s="10"/>
-      <c r="L281" s="10"/>
+      <c r="G281" s="7"/>
+      <c r="K281" s="9"/>
+      <c r="L281" s="9"/>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
@@ -5330,9 +5336,9 @@
       <c r="E282" s="4">
         <v>303.363</v>
       </c>
-      <c r="G282" s="8"/>
-      <c r="K282" s="10"/>
-      <c r="L282" s="10"/>
+      <c r="G282" s="7"/>
+      <c r="K282" s="9"/>
+      <c r="L282" s="9"/>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
@@ -5350,9 +5356,9 @@
       <c r="E283" s="4">
         <v>304.12700000000001</v>
       </c>
-      <c r="G283" s="8"/>
-      <c r="K283" s="10"/>
-      <c r="L283" s="10"/>
+      <c r="G283" s="7"/>
+      <c r="K283" s="9"/>
+      <c r="L283" s="9"/>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
@@ -5370,9 +5376,9 @@
       <c r="E284" s="4">
         <v>305.10899999999998</v>
       </c>
-      <c r="G284" s="8"/>
-      <c r="K284" s="10"/>
-      <c r="L284" s="10"/>
+      <c r="G284" s="7"/>
+      <c r="K284" s="9"/>
+      <c r="L284" s="9"/>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
@@ -5390,9 +5396,9 @@
       <c r="E285" s="4">
         <v>305.69099999999997</v>
       </c>
-      <c r="G285" s="8"/>
-      <c r="K285" s="10"/>
-      <c r="L285" s="10"/>
+      <c r="G285" s="7"/>
+      <c r="K285" s="9"/>
+      <c r="L285" s="9"/>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
@@ -5410,9 +5416,9 @@
       <c r="E286" s="4">
         <v>307.02600000000001</v>
       </c>
-      <c r="G286" s="8"/>
-      <c r="K286" s="10"/>
-      <c r="L286" s="10"/>
+      <c r="G286" s="7"/>
+      <c r="K286" s="9"/>
+      <c r="L286" s="9"/>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
@@ -5430,9 +5436,9 @@
       <c r="E287" s="4">
         <v>307.78899999999999</v>
       </c>
-      <c r="G287" s="8"/>
-      <c r="K287" s="10"/>
-      <c r="L287" s="10"/>
+      <c r="G287" s="7"/>
+      <c r="K287" s="9"/>
+      <c r="L287" s="9"/>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
@@ -5450,9 +5456,9 @@
       <c r="E288" s="4">
         <v>307.67099999999999</v>
       </c>
-      <c r="G288" s="8"/>
-      <c r="K288" s="10"/>
-      <c r="L288" s="10"/>
+      <c r="G288" s="7"/>
+      <c r="K288" s="9"/>
+      <c r="L288" s="9"/>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
@@ -5470,11 +5476,11 @@
       <c r="E289" s="4">
         <v>307.05099999999999</v>
       </c>
-      <c r="G289" s="8"/>
-      <c r="H289" s="9"/>
-      <c r="I289" s="9"/>
-      <c r="K289" s="11"/>
-      <c r="L289" s="10"/>
+      <c r="G289" s="7"/>
+      <c r="H289" s="8"/>
+      <c r="I289" s="8"/>
+      <c r="K289" s="10"/>
+      <c r="L289" s="9"/>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
@@ -5501,7 +5507,7 @@
         <v>138.97999999999999</v>
       </c>
       <c r="C291" s="4">
-        <v>79.149545454545446</v>
+        <v>80.12</v>
       </c>
       <c r="D291" s="4">
         <v>101.483</v>
@@ -5518,7 +5524,7 @@
         <v>140.49</v>
       </c>
       <c r="C292" s="4">
-        <v>81.716190476190476</v>
+        <v>83.48</v>
       </c>
       <c r="D292" s="4">
         <v>102.72669999999999</v>
@@ -5535,7 +5541,7 @@
         <v>141.47999999999999</v>
       </c>
       <c r="C293" s="4">
-        <v>84.799523809523805</v>
+        <v>85.41</v>
       </c>
       <c r="D293" s="4">
         <v>102.51860000000001</v>
@@ -5552,7 +5558,7 @@
         <v>142.32</v>
       </c>
       <c r="C294" s="4">
-        <v>89</v>
+        <v>89.94</v>
       </c>
       <c r="D294" s="4">
         <v>102.35680000000001</v>
@@ -5569,10 +5575,10 @@
         <v>142.91999999999999</v>
       </c>
       <c r="C295" s="4">
-        <v>82.996521739130415</v>
+        <v>81.75</v>
       </c>
       <c r="D295" s="4">
-        <v>103.0711</v>
+        <v>102.97969999999999</v>
       </c>
       <c r="E295" s="4">
         <v>314.06900000000002</v>
@@ -5586,10 +5592,10 @@
         <v>143.38</v>
       </c>
       <c r="C296" s="4">
-        <v>82.998500000000007</v>
+        <v>82.25</v>
       </c>
       <c r="D296" s="4">
-        <v>103.22580000000001</v>
+        <v>103.2534</v>
       </c>
       <c r="E296" s="4">
         <v>314.17500000000001</v>
@@ -5603,10 +5609,10 @@
         <v>143.66999999999999</v>
       </c>
       <c r="C297" s="4">
-        <v>83.87913043478261</v>
+        <v>85.15</v>
       </c>
       <c r="D297" s="4">
-        <v>102.58629999999999</v>
+        <v>102.5192</v>
       </c>
       <c r="E297" s="4">
         <v>314.54000000000002</v>
@@ -5620,10 +5626,10 @@
         <v>143.66999999999999</v>
       </c>
       <c r="C298" s="4">
-        <v>78.875000000000014</v>
+        <v>80.36</v>
       </c>
       <c r="D298" s="4">
-        <v>102.9329</v>
+        <v>103.0196</v>
       </c>
       <c r="E298" s="4">
         <v>314.79599999999999</v>
@@ -5637,10 +5643,10 @@
         <v>144.02000000000001</v>
       </c>
       <c r="C299" s="4">
-        <v>72.870952380952374</v>
+        <v>74.02</v>
       </c>
       <c r="D299" s="4">
-        <v>102.6418</v>
+        <v>102.5954</v>
       </c>
       <c r="E299" s="4">
         <v>315.30099999999999</v>
@@ -5651,17 +5657,135 @@
         <v>45566</v>
       </c>
       <c r="B300" s="4">
-        <v>144.26483400000001</v>
+        <v>143.83000000000001</v>
       </c>
       <c r="C300" s="4">
-        <v>75.376956521739132</v>
+        <v>75.63</v>
       </c>
       <c r="D300" s="4">
-        <f>+D288*(1+2%)</f>
-        <v>104.619666</v>
+        <v>102.21380000000001</v>
       </c>
       <c r="E300" s="4">
         <v>315.66399999999999</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A301" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B301" s="4">
+        <v>144.22</v>
+      </c>
+      <c r="C301" s="4">
+        <v>74.349999999999994</v>
+      </c>
+      <c r="D301" s="4">
+        <v>101.9503</v>
+      </c>
+      <c r="E301" s="4">
+        <v>315.49299999999999</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A302" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B302" s="4">
+        <v>144.88</v>
+      </c>
+      <c r="C302" s="4">
+        <v>73.86</v>
+      </c>
+      <c r="D302" s="4">
+        <v>103.04470000000001</v>
+      </c>
+      <c r="E302" s="4">
+        <v>315.60500000000002</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A303" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B303" s="4">
+        <v>146.24</v>
+      </c>
+      <c r="C303" s="4">
+        <v>79.27</v>
+      </c>
+      <c r="D303" s="4">
+        <v>102.93429999999999</v>
+      </c>
+      <c r="E303" s="4">
+        <v>317.67099999999999</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A304" s="1">
+        <v>45689</v>
+      </c>
+      <c r="B304" s="4">
+        <v>147.9</v>
+      </c>
+      <c r="C304" s="4">
+        <v>75.44</v>
+      </c>
+      <c r="D304" s="4">
+        <v>104.0003</v>
+      </c>
+      <c r="E304" s="4">
+        <v>319.08199999999999</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A305" s="1">
+        <v>45717</v>
+      </c>
+      <c r="B305" s="4">
+        <v>148.68</v>
+      </c>
+      <c r="C305" s="4">
+        <v>72.73</v>
+      </c>
+      <c r="D305" s="4">
+        <v>103.7483</v>
+      </c>
+      <c r="E305" s="4">
+        <v>319.79899999999998</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A306" s="1">
+        <v>45748</v>
+      </c>
+      <c r="B306" s="4">
+        <v>149.66</v>
+      </c>
+      <c r="C306" s="4">
+        <v>68.13</v>
+      </c>
+      <c r="D306" s="4">
+        <v>103.8216</v>
+      </c>
+      <c r="E306" s="4">
+        <v>320.79500000000002</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A307" s="1">
+        <v>45778</v>
+      </c>
+      <c r="B307" s="4">
+        <v>150.13999999999999</v>
+      </c>
+      <c r="C307" s="4">
+        <v>64.45</v>
+      </c>
+      <c r="D307" s="4">
+        <v>103.59480000000001</v>
+      </c>
+      <c r="E307" s="4">
+        <v>321.46499999999997</v>
       </c>
     </row>
   </sheetData>
@@ -5681,26 +5805,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C921DE1D-2686-44DF-B218-59946BA2C5A6}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:D4"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
+      <c r="B1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -5719,219 +5843,275 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45566</v>
-      </c>
-      <c r="B4" s="12">
-        <v>75.376956521739132</v>
-      </c>
-      <c r="C4" s="7">
-        <v>104.619666</v>
-      </c>
-      <c r="D4" s="7">
-        <v>315.66399999999999</v>
+        <v>45809</v>
+      </c>
+      <c r="B4" s="11">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6">
+        <v>104.3095</v>
+      </c>
+      <c r="D4" s="6">
+        <v>325.8784905678454</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B5" s="6">
-        <v>76</v>
-      </c>
-      <c r="C5" s="7">
-        <v>103.09699999999999</v>
-      </c>
-      <c r="D5" s="7">
-        <v>314.26484038808667</v>
+        <v>45839</v>
+      </c>
+      <c r="B5" s="11">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6">
+        <v>104.2833</v>
+      </c>
+      <c r="D5" s="6">
+        <v>325.79886403500382</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45627</v>
-      </c>
-      <c r="B6" s="6">
-        <v>77</v>
-      </c>
-      <c r="C6" s="7">
-        <v>103.1674</v>
-      </c>
-      <c r="D6" s="7">
-        <v>313.66537553815164</v>
+        <v>45870</v>
+      </c>
+      <c r="B6" s="11">
+        <v>62</v>
+      </c>
+      <c r="C6" s="6">
+        <v>104.2214</v>
+      </c>
+      <c r="D6" s="6">
+        <v>326.0687133724465</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45658</v>
-      </c>
-      <c r="B7" s="6">
-        <v>77</v>
-      </c>
-      <c r="C7" s="7">
-        <v>103.1811</v>
-      </c>
-      <c r="D7" s="7">
-        <v>314.94067908842851</v>
+        <v>45901</v>
+      </c>
+      <c r="B7" s="11">
+        <v>62</v>
+      </c>
+      <c r="C7" s="6">
+        <v>104.11360000000001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>326.51139956804968</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>45689</v>
-      </c>
-      <c r="B8" s="6">
-        <v>78</v>
-      </c>
-      <c r="C8" s="7">
-        <v>103.2642</v>
-      </c>
-      <c r="D8" s="7">
-        <v>315.95988335980252</v>
+        <v>45931</v>
+      </c>
+      <c r="B8" s="11">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6">
+        <v>103.8789</v>
+      </c>
+      <c r="D8" s="6">
+        <v>327.0313010761684</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45717</v>
-      </c>
-      <c r="B9" s="6">
-        <v>79</v>
-      </c>
-      <c r="C9" s="7">
-        <v>103.37069999999999</v>
-      </c>
-      <c r="D9" s="7">
-        <v>317.26030946545814</v>
+        <v>45962</v>
+      </c>
+      <c r="B9" s="11">
+        <v>61</v>
+      </c>
+      <c r="C9" s="6">
+        <v>103.7397</v>
+      </c>
+      <c r="D9" s="6">
+        <v>326.64889564858794</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>45748</v>
-      </c>
-      <c r="B10" s="6">
-        <v>78</v>
-      </c>
-      <c r="C10" s="7">
-        <v>103.44782895813384</v>
-      </c>
-      <c r="D10" s="7">
-        <v>317.86429419776698</v>
+        <v>45992</v>
+      </c>
+      <c r="B10" s="11">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6">
+        <v>103.6151</v>
+      </c>
+      <c r="D10" s="6">
+        <v>326.25428260595783</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45778</v>
-      </c>
-      <c r="B11" s="6">
-        <v>78</v>
-      </c>
-      <c r="C11" s="7">
-        <v>103.42717495000757</v>
-      </c>
-      <c r="D11" s="7">
-        <v>318.87371173820742</v>
+        <v>46023</v>
+      </c>
+      <c r="B11" s="11">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6">
+        <v>103.4579</v>
+      </c>
+      <c r="D11" s="6">
+        <v>327.52231932833155</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>45809</v>
-      </c>
-      <c r="B12" s="6">
-        <v>77</v>
-      </c>
-      <c r="C12" s="7">
-        <v>103.77958539501432</v>
-      </c>
-      <c r="D12" s="7">
-        <v>319.71355010717173</v>
+        <v>46054</v>
+      </c>
+      <c r="B12" s="11">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6">
+        <v>103.398</v>
+      </c>
+      <c r="D12" s="6">
+        <v>328.87952119959346</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>45839</v>
-      </c>
-      <c r="B13" s="6">
-        <v>76</v>
-      </c>
-      <c r="C13" s="7">
-        <v>104.0940249469727</v>
-      </c>
-      <c r="D13" s="7">
-        <v>320.32189234979307</v>
+        <v>46082</v>
+      </c>
+      <c r="B13" s="11">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6">
+        <v>103.38809999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>330.35827539946496</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45870</v>
-      </c>
-      <c r="B14" s="6">
-        <v>76</v>
-      </c>
-      <c r="C14" s="7">
-        <v>103.89822157983068</v>
-      </c>
-      <c r="D14" s="7">
-        <v>320.54633012119535</v>
+        <v>46113</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="6">
+        <v>103.50190000000001</v>
+      </c>
+      <c r="D14" s="6">
+        <v>328.56104935204536</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>45901</v>
-      </c>
-      <c r="B15" s="6">
-        <v>75</v>
-      </c>
-      <c r="C15" s="7">
-        <v>103.8518879862369</v>
-      </c>
-      <c r="D15" s="7">
-        <v>321.00462501827212</v>
+        <v>46143</v>
+      </c>
+      <c r="B15" s="11">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6">
+        <v>103.5369</v>
+      </c>
+      <c r="D15" s="6">
+        <v>328.6284137872027</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B16" s="6">
-        <v>74</v>
-      </c>
-      <c r="C16" s="7">
-        <v>103.58895719647614</v>
-      </c>
-      <c r="D16" s="7">
-        <v>321.62969326537109</v>
+        <v>46174</v>
+      </c>
+      <c r="B16" s="11">
+        <v>60</v>
+      </c>
+      <c r="C16" s="6">
+        <v>103.5668</v>
+      </c>
+      <c r="D16" s="6">
+        <v>332.84915400423472</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45962</v>
-      </c>
-      <c r="B17" s="6">
-        <v>73</v>
-      </c>
-      <c r="C17" s="7">
-        <v>104.5307</v>
-      </c>
-      <c r="D17" s="7">
-        <v>320.26143804151621</v>
+        <v>46204</v>
+      </c>
+      <c r="B17" s="11">
+        <v>59</v>
+      </c>
+      <c r="C17" s="6">
+        <v>103.5582</v>
+      </c>
+      <c r="D17" s="6">
+        <v>333.3641907158302</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>45992</v>
-      </c>
-      <c r="B18" s="6">
-        <v>72</v>
-      </c>
-      <c r="C18" s="7">
-        <v>104.74600000000001</v>
-      </c>
-      <c r="D18" s="7">
-        <v>319.68083288311925</v>
+        <v>46235</v>
+      </c>
+      <c r="B18" s="11">
+        <v>59</v>
+      </c>
+      <c r="C18" s="6">
+        <v>103.60290000000001</v>
+      </c>
+      <c r="D18" s="6">
+        <v>333.59801887365461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>46266</v>
+      </c>
+      <c r="B19" s="11">
+        <v>59</v>
+      </c>
+      <c r="C19" s="6">
+        <v>103.6675</v>
+      </c>
+      <c r="D19" s="6">
+        <v>333.92558114473201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>46296</v>
+      </c>
+      <c r="B20" s="11">
+        <v>58</v>
+      </c>
+      <c r="C20" s="6">
+        <v>103.7877</v>
+      </c>
+      <c r="D20" s="6">
+        <v>334.24918764878117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>46327</v>
+      </c>
+      <c r="B21" s="11">
+        <v>58</v>
+      </c>
+      <c r="C21" s="6">
+        <v>103.8653</v>
+      </c>
+      <c r="D21" s="6">
+        <v>333.56842823203743</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>46357</v>
+      </c>
+      <c r="B22" s="11">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6">
+        <v>103.93600000000001</v>
+      </c>
+      <c r="D22" s="6">
+        <v>332.79427985724328</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="https://fred.stlouisfed.org/series/INDPRO" xr:uid="{3F4A283C-523A-4303-8C54-CD8CFEA29BE1}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{F8B9ED1B-AE37-4AC9-9547-EE95DD73D871}"/>
-    <hyperlink ref="D1" r:id="rId3" xr:uid="{66C97603-7098-4051-9CEC-484FE240E28A}"/>
+    <hyperlink ref="D1" r:id="rId1" display="https://data.bls.gov/timeseries/CUUR0000SA0?years_option=all_years" xr:uid="{4D1AFAAF-6C13-415E-A948-7F0168239501}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{45067D20-6E3E-437E-BA90-66A9ADC9F071}"/>
+    <hyperlink ref="B1" r:id="rId3" display="https://fred.stlouisfed.org/series/MCOILBRENTEU" xr:uid="{E4CF1300-5928-4F83-8E1A-6ED4176EF7E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Update files for taking latest chages - 251203
</commit_message>
<xml_diff>
--- a/Base_Modelo_ARIMAX.xlsx
+++ b/Base_Modelo_ARIMAX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\repos\ARIMAX_Conditional_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54B4A7D-97D2-4F38-86A5-19668700896E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A101A6-84BC-4D5B-8795-74A04518A3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{907D08FB-30E1-4FC8-8C13-8C04F9DAF021}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -513,21 +513,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88848EC6-D3A9-432A-B99B-25298BB184AA}">
-  <dimension ref="A1:L307"/>
+  <dimension ref="A1:L312"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B289" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E323" sqref="E323"/>
+      <selection pane="bottomRight" activeCell="G316" sqref="G316"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -544,7 +544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -561,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>36526</v>
       </c>
@@ -578,7 +578,7 @@
         <v>168.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>36557</v>
       </c>
@@ -595,7 +595,7 @@
         <v>169.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>36586</v>
       </c>
@@ -612,7 +612,7 @@
         <v>171.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>36617</v>
       </c>
@@ -629,7 +629,7 @@
         <v>171.3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>36647</v>
       </c>
@@ -646,7 +646,7 @@
         <v>171.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>36678</v>
       </c>
@@ -663,7 +663,7 @@
         <v>172.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>36708</v>
       </c>
@@ -680,7 +680,7 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>36739</v>
       </c>
@@ -697,7 +697,7 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>36770</v>
       </c>
@@ -714,7 +714,7 @@
         <v>173.7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>36800</v>
       </c>
@@ -731,7 +731,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>36831</v>
       </c>
@@ -748,7 +748,7 @@
         <v>174.1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>36861</v>
       </c>
@@ -765,7 +765,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>36892</v>
       </c>
@@ -782,7 +782,7 @@
         <v>175.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>36923</v>
       </c>
@@ -799,7 +799,7 @@
         <v>175.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>36951</v>
       </c>
@@ -816,7 +816,7 @@
         <v>176.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>36982</v>
       </c>
@@ -833,7 +833,7 @@
         <v>176.9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>37012</v>
       </c>
@@ -850,7 +850,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>37043</v>
       </c>
@@ -867,7 +867,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>37073</v>
       </c>
@@ -884,7 +884,7 @@
         <v>177.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>37104</v>
       </c>
@@ -901,7 +901,7 @@
         <v>177.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>37135</v>
       </c>
@@ -918,7 +918,7 @@
         <v>178.3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>37165</v>
       </c>
@@ -935,7 +935,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>37196</v>
       </c>
@@ -952,7 +952,7 @@
         <v>177.4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>37226</v>
       </c>
@@ -969,7 +969,7 @@
         <v>176.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>37257</v>
       </c>
@@ -986,7 +986,7 @@
         <v>177.1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>37288</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>177.8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>37316</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>178.8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>37347</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>179.8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>37377</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>179.8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>37408</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>179.9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>37438</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>180.1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>37469</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>180.7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>37500</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>37530</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>181.3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>37561</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>181.3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37591</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>180.9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37622</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>181.7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>37653</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>183.1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>37681</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>184.2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>37712</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>183.8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>37742</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>183.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>37773</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>183.7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>37803</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>183.9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>37834</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>184.6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>37865</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>185.2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>37895</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>37926</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>184.5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>37956</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>184.3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>37987</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>185.2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>38018</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>186.2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>38047</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>187.4</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>38078</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>38108</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>189.1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>38139</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>189.7</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>38169</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>189.4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>38200</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>189.5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>38231</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>189.9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>38261</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>190.9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>38292</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>38322</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>190.3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>38353</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>190.7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>38384</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>191.8</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>38412</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>193.3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>38443</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>194.6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>38473</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>194.4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>38504</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>194.5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>38534</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>195.4</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>38565</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>196.4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>38596</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>198.8</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>38626</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>199.2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>38657</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>197.6</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>38687</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>196.8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>38718</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>198.3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>38749</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>198.7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>38777</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>199.8</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>38808</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>201.5</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>38838</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>202.5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>38869</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>202.9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>38899</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>203.5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>38930</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>203.9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>38961</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>202.9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>38991</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>201.8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>39022</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>201.5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>39052</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>201.8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>39083</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>202.416</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>39114</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>203.499</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>39142</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>205.352</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>39173</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>206.68600000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>39203</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>207.94900000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>39234</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>208.352</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>39264</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>208.29900000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>39295</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>207.917</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>39326</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>208.49</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>39356</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>208.93600000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>39387</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>210.17699999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>39417</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>210.036</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>39448</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>211.08</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>39479</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>211.69300000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>39508</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>213.52799999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>39539</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>214.82300000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>39569</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>216.63200000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>39600</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>218.815</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>39630</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>219.964</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>39661</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>219.08600000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>39692</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>218.78299999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>39722</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>216.57300000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>39753</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>212.42500000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>39783</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>210.22800000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>39814</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>211.143</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>39845</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>212.19300000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>39873</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>212.709</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>39904</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>213.24</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>39934</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>213.85599999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>39965</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>215.69300000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>39995</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>215.351</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>40026</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>215.834</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>40057</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>215.96899999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>40087</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>216.17699999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>40118</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>216.33</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>40148</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>215.94900000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>40179</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>216.68700000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>40210</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>216.74100000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>40238</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>217.631</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>40269</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>218.00899999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>40299</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>218.178</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>40330</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>217.965</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>40360</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>218.011</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>40391</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>218.31200000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>40422</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>218.43899999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>40452</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>218.71100000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>40483</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>218.803</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>40513</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>219.179</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>40544</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>220.22300000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>40575</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>221.309</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>40603</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>223.46700000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>40634</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>224.90600000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>40664</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>225.964</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>40695</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>225.72200000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>40725</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>225.922</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>40756</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>226.54499999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>40787</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>226.88900000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>40817</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>226.42099999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>40848</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>226.23</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>40878</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>225.672</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>40909</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>226.66499999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>40940</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>227.66300000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>40969</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>229.392</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>41000</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>230.08500000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>41030</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>229.815</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>41061</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>229.47800000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>41091</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>229.10400000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>41122</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>230.37899999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>41153</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>231.40700000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>41183</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>231.31700000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>41214</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>230.221</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>41244</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>229.601</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>41275</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>230.28</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>41306</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>232.166</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>41334</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>232.773</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>41365</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>232.53100000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>41395</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>232.94499999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>41426</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>233.50399999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>41456</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>233.596</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>41487</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>233.87700000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>41518</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>234.149</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>41548</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>233.54599999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>41579</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>233.06899999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>41609</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>233.04900000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>41640</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>233.916</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>41671</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>234.78100000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>41699</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>236.29300000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>41730</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>237.072</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>41760</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>237.9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>41791</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>238.34299999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>41821</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>238.25</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>41852</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>237.852</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>41883</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>238.03100000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>41913</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>237.43299999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>41944</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>236.15100000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>41974</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>234.81200000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>42005</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>233.70699999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>42036</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>234.72200000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>42064</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>236.119</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>42095</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>236.59899999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>42125</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>237.80500000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>42156</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>238.63800000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>42186</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>238.654</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>42217</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>238.316</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>42248</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>237.94499999999999</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>42278</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>237.83799999999999</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>42309</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>237.33600000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>42339</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>236.52500000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>42370</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>236.916</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>42401</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>237.11099999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>42430</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>238.13200000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>42461</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>239.261</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>42491</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>240.22900000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>42522</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>241.018</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>42552</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>240.62799999999999</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>42583</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>240.84899999999999</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>42614</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>241.428</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>42644</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>241.72900000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>42675</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>241.35300000000001</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>42705</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>241.43199999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>42736</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>242.839</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>42767</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>243.60300000000001</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>42795</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>243.80099999999999</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>42826</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>244.524</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>42856</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>244.733</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>42887</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>244.95500000000001</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>42917</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>244.786</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>42948</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>245.51900000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>42979</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>246.81899999999999</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>43009</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>246.66300000000001</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>43040</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>246.66900000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>43070</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>246.524</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>43101</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>247.86699999999999</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>43132</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>248.99100000000001</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>43160</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>249.554</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>43191</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>250.54599999999999</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>43221</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>251.58799999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>43252</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>251.989</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>43282</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>252.006</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>43313</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>252.14599999999999</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>43344</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>252.43899999999999</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>43374</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>252.88499999999999</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>43405</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>252.03800000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>43435</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>251.233</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>43466</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>251.71199999999999</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>43497</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>252.77600000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>43525</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>254.202</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>43556</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>255.548</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>43586</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>256.09199999999998</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>43617</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>256.14299999999997</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>43647</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>256.57100000000003</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>43678</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>256.55799999999999</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>43709</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>256.75900000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>43739</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>257.346</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>43770</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>257.20800000000003</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>43800</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>256.97399999999999</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>43831</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>257.971</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>43862</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>258.678</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>43891</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>258.11500000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>43922</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>256.38900000000001</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>43952</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>256.39400000000001</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>43983</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>257.79700000000003</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>44013</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>259.101</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>44044</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>259.91800000000001</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>44075</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>260.27999999999997</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>44105</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>260.38799999999998</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>44136</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>260.22899999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>44166</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>260.47399999999999</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>44197</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>261.58199999999999</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>44228</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>263.01400000000001</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>44256</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>264.87700000000001</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>44287</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>267.05399999999997</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>44317</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>269.19499999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>44348</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>271.69600000000003</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>44378</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>273.00299999999999</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
         <v>44409</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>273.56700000000001</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
         <v>44440</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>274.31</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
         <v>44470</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>276.589</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>44501</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>277.94799999999998</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>44531</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>278.80200000000002</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>44562</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>281.14800000000002</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
         <v>44593</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>283.71600000000001</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
         <v>44621</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>287.50400000000002</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
         <v>44652</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>289.10899999999998</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
         <v>44682</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>292.29599999999999</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
         <v>44713</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>296.31099999999998</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
         <v>44743</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>296.27600000000001</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
         <v>44774</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>296.17099999999999</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
         <v>44805</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>296.80799999999999</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
         <v>44835</v>
       </c>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="K276" s="9"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
         <v>44866</v>
       </c>
@@ -5240,7 +5240,7 @@
       <c r="K277" s="9"/>
       <c r="L277" s="9"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
         <v>44896</v>
       </c>
@@ -5260,7 +5260,7 @@
       <c r="K278" s="9"/>
       <c r="L278" s="9"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
         <v>44927</v>
       </c>
@@ -5280,7 +5280,7 @@
       <c r="K279" s="9"/>
       <c r="L279" s="9"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
         <v>44958</v>
       </c>
@@ -5300,7 +5300,7 @@
       <c r="K280" s="9"/>
       <c r="L280" s="9"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
         <v>44986</v>
       </c>
@@ -5320,7 +5320,7 @@
       <c r="K281" s="9"/>
       <c r="L281" s="9"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
         <v>45017</v>
       </c>
@@ -5340,7 +5340,7 @@
       <c r="K282" s="9"/>
       <c r="L282" s="9"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
         <v>45047</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="K283" s="9"/>
       <c r="L283" s="9"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
         <v>45078</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="K284" s="9"/>
       <c r="L284" s="9"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
         <v>45108</v>
       </c>
@@ -5400,7 +5400,7 @@
       <c r="K285" s="9"/>
       <c r="L285" s="9"/>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
         <v>45139</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="K286" s="9"/>
       <c r="L286" s="9"/>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
         <v>45170</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="K287" s="9"/>
       <c r="L287" s="9"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
         <v>45200</v>
       </c>
@@ -5460,7 +5460,7 @@
       <c r="K288" s="9"/>
       <c r="L288" s="9"/>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
         <v>45231</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="K289" s="10"/>
       <c r="L289" s="9"/>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
         <v>45261</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>306.74599999999998</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
         <v>45292</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>308.41699999999997</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
         <v>45323</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>310.32600000000002</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
         <v>45352</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>312.33199999999999</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
         <v>45383</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>313.548</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
         <v>45413</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>314.06900000000002</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
         <v>45444</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>314.17500000000001</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
         <v>45474</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>314.54000000000002</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
         <v>45505</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>314.79599999999999</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
         <v>45536</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>315.30099999999999</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
         <v>45566</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>315.66399999999999</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
         <v>45597</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>315.49299999999999</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" s="1">
         <v>45627</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>315.60500000000002</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" s="1">
         <v>45658</v>
       </c>
@@ -5714,13 +5714,13 @@
         <v>79.27</v>
       </c>
       <c r="D303" s="4">
-        <v>102.93429999999999</v>
+        <v>102.8805</v>
       </c>
       <c r="E303" s="4">
         <v>317.67099999999999</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" s="1">
         <v>45689</v>
       </c>
@@ -5731,13 +5731,13 @@
         <v>75.44</v>
       </c>
       <c r="D304" s="4">
-        <v>104.0003</v>
+        <v>103.87050000000001</v>
       </c>
       <c r="E304" s="4">
         <v>319.08199999999999</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="1">
         <v>45717</v>
       </c>
@@ -5748,13 +5748,13 @@
         <v>72.73</v>
       </c>
       <c r="D305" s="4">
-        <v>103.7483</v>
+        <v>103.5408</v>
       </c>
       <c r="E305" s="4">
         <v>319.79899999999998</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="1">
         <v>45748</v>
       </c>
@@ -5765,13 +5765,13 @@
         <v>68.13</v>
       </c>
       <c r="D306" s="4">
-        <v>103.8216</v>
+        <v>103.6224</v>
       </c>
       <c r="E306" s="4">
         <v>320.79500000000002</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="1">
         <v>45778</v>
       </c>
@@ -5782,10 +5782,95 @@
         <v>64.45</v>
       </c>
       <c r="D307" s="4">
-        <v>103.59480000000001</v>
+        <v>103.657</v>
       </c>
       <c r="E307" s="4">
         <v>321.46499999999997</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A308" s="1">
+        <v>45809</v>
+      </c>
+      <c r="B308" s="4">
+        <v>150.30000000000001</v>
+      </c>
+      <c r="C308" s="4">
+        <v>71.44</v>
+      </c>
+      <c r="D308" s="4">
+        <v>104.2115</v>
+      </c>
+      <c r="E308" s="4">
+        <v>322.56099999999998</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A309" s="1">
+        <v>45839</v>
+      </c>
+      <c r="B309" s="4">
+        <v>150.71</v>
+      </c>
+      <c r="C309" s="4">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="D309" s="4">
+        <v>103.8194</v>
+      </c>
+      <c r="E309" s="4">
+        <v>323.048</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A310" s="1">
+        <v>45870</v>
+      </c>
+      <c r="B310" s="4">
+        <v>150.99</v>
+      </c>
+      <c r="C310" s="4">
+        <v>67.87</v>
+      </c>
+      <c r="D310" s="4">
+        <v>103.9203</v>
+      </c>
+      <c r="E310" s="4">
+        <v>323.976</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A311" s="1">
+        <v>45901</v>
+      </c>
+      <c r="B311" s="4">
+        <v>151.47999999999999</v>
+      </c>
+      <c r="C311" s="4">
+        <v>67.989999999999995</v>
+      </c>
+      <c r="D311" s="4">
+        <v>103.87066667000001</v>
+      </c>
+      <c r="E311" s="4">
+        <v>324.8</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A312" s="1">
+        <v>45931</v>
+      </c>
+      <c r="B312" s="4">
+        <v>151.76</v>
+      </c>
+      <c r="C312" s="4">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="D312" s="4">
+        <v>103.67265184999999</v>
+      </c>
+      <c r="E312" s="4">
+        <v>324.97297036999998</v>
       </c>
     </row>
   </sheetData>
@@ -5805,18 +5890,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C921DE1D-2686-44DF-B218-59946BA2C5A6}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="12" t="s">
         <v>10</v>
       </c>
@@ -5827,7 +5912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -5841,270 +5926,200 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>45809</v>
+        <v>45962</v>
       </c>
       <c r="B4" s="11">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="6">
-        <v>104.3095</v>
+        <v>103.5446</v>
       </c>
       <c r="D4" s="6">
-        <v>325.8784905678454</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>325.77719999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45839</v>
+        <v>45992</v>
       </c>
       <c r="B5" s="11">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6">
-        <v>104.2833</v>
+        <v>103.416</v>
       </c>
       <c r="D5" s="6">
-        <v>325.79886403500382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>326.55840000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45870</v>
+        <v>46023</v>
       </c>
       <c r="B6" s="11">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" s="6">
-        <v>104.2214</v>
+        <v>103.2334</v>
       </c>
       <c r="D6" s="6">
-        <v>326.0687133724465</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>327.36860000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45901</v>
+        <v>46054</v>
       </c>
       <c r="B7" s="11">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6">
-        <v>104.11360000000001</v>
+        <v>103.14400000000001</v>
       </c>
       <c r="D7" s="6">
-        <v>326.51139956804968</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>328.06479999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="B8" s="11">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6">
-        <v>103.8789</v>
+        <v>103.0942</v>
       </c>
       <c r="D8" s="6">
-        <v>327.0313010761684</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>328.69920000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45962</v>
+        <v>46113</v>
       </c>
       <c r="B9" s="11">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6">
-        <v>103.7397</v>
+        <v>103.09690000000001</v>
       </c>
       <c r="D9" s="6">
-        <v>326.64889564858794</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>329.14479999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45992</v>
+        <v>46143</v>
       </c>
       <c r="B10" s="11">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C10" s="6">
-        <v>103.6151</v>
+        <v>103.1169</v>
       </c>
       <c r="D10" s="6">
-        <v>326.25428260595783</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>329.75040000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>46023</v>
+        <v>46174</v>
       </c>
       <c r="B11" s="11">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6">
-        <v>103.4579</v>
+        <v>103.16719999999999</v>
       </c>
       <c r="D11" s="6">
-        <v>327.52231932833155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>330.38900000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>46054</v>
+        <v>46204</v>
       </c>
       <c r="B12" s="11">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C12" s="6">
-        <v>103.398</v>
+        <v>103.2869</v>
       </c>
       <c r="D12" s="6">
-        <v>328.87952119959346</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>331.12799999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>46082</v>
+        <v>46235</v>
       </c>
       <c r="B13" s="11">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C13" s="6">
-        <v>103.38809999999999</v>
+        <v>103.36799999999999</v>
       </c>
       <c r="D13" s="6">
-        <v>330.35827539946496</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>331.78250000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>46113</v>
+        <v>46266</v>
       </c>
       <c r="B14" s="11">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C14" s="6">
-        <v>103.50190000000001</v>
+        <v>103.44970000000001</v>
       </c>
       <c r="D14" s="6">
-        <v>328.56104935204536</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>332.41989999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>46143</v>
+        <v>46296</v>
       </c>
       <c r="B15" s="11">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C15" s="6">
-        <v>103.5369</v>
+        <v>103.55629999999999</v>
       </c>
       <c r="D15" s="6">
-        <v>328.6284137872027</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>333.08159999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>46174</v>
+        <v>46327</v>
       </c>
       <c r="B16" s="11">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="6">
-        <v>103.5668</v>
+        <v>103.62130000000001</v>
       </c>
       <c r="D16" s="6">
-        <v>332.84915400423472</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>333.6533</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>46204</v>
+        <v>46357</v>
       </c>
       <c r="B17" s="11">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6">
-        <v>103.5582</v>
+        <v>103.66889999999999</v>
       </c>
       <c r="D17" s="6">
-        <v>333.3641907158302</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>46235</v>
-      </c>
-      <c r="B18" s="11">
-        <v>59</v>
-      </c>
-      <c r="C18" s="6">
-        <v>103.60290000000001</v>
-      </c>
-      <c r="D18" s="6">
-        <v>333.59801887365461</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>46266</v>
-      </c>
-      <c r="B19" s="11">
-        <v>59</v>
-      </c>
-      <c r="C19" s="6">
-        <v>103.6675</v>
-      </c>
-      <c r="D19" s="6">
-        <v>333.92558114473201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>46296</v>
-      </c>
-      <c r="B20" s="11">
-        <v>58</v>
-      </c>
-      <c r="C20" s="6">
-        <v>103.7877</v>
-      </c>
-      <c r="D20" s="6">
-        <v>334.24918764878117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>46327</v>
-      </c>
-      <c r="B21" s="11">
-        <v>58</v>
-      </c>
-      <c r="C21" s="6">
-        <v>103.8653</v>
-      </c>
-      <c r="D21" s="6">
-        <v>333.56842823203743</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>46357</v>
-      </c>
-      <c r="B22" s="11">
-        <v>58</v>
-      </c>
-      <c r="C22" s="6">
-        <v>103.93600000000001</v>
-      </c>
-      <c r="D22" s="6">
-        <v>332.79427985724328</v>
+        <v>334.17660000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>